<commit_message>
unique values for procs and comm
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -56,7 +56,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -85,12 +85,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00DDD9C4"/>
         <bgColor rgb="00DDD9C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D9D9D9"/>
-        <bgColor rgb="00D9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -132,7 +126,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9549,7 +9543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:I278"/>
+  <dimension ref="B1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9718,1869 +9712,245 @@
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>iip_heat_proc</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>pri_coal</t>
+          <t>iip_steel_crudesteel</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t>iip_coke</t>
+          <t>iip_steel_sponge_iron</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="C15" t="inlineStr">
         <is>
-          <t>sec_heavy_fuel_oil</t>
+          <t>iip_steel_scrap</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="C16" t="inlineStr">
         <is>
-          <t>iip_steel_sinter</t>
+          <t>iip_steel_iron_ore</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>iip_steel_raw_iron</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="C18" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>iip_steel_iron_pellets</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="C19" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>sec_biogas</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>sec_heating_oil</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="C21" t="inlineStr">
         <is>
-          <t>pri_coal</t>
+          <t>sec_H2</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="C22" t="inlineStr">
         <is>
-          <t>iip_coke</t>
+          <t>pri_natural_gas</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="C23" t="inlineStr">
         <is>
-          <t>sec_heavy_fuel_oil</t>
+          <t>sec_natural_gas_syn</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="C24" t="inlineStr">
         <is>
-          <t>iip_steel_sinter</t>
+          <t>pri_biomass</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="C25" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>pri_waste</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="C26" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>pri_geoth_heat</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="C27" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>pri_hydro_energy</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>pri_uran</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="C29" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>pri_deuterium</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="C30" t="inlineStr">
         <is>
-          <t>iip_heat_proc</t>
+          <t>pri_solar_radiation</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="C31" t="inlineStr">
         <is>
-          <t>iip_steel_crudesteel</t>
+          <t>sec_elec</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="C32" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>pri_wind_energy_off</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="C33" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>pri_wind_energy_on</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="C34" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>sec_heat_low</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="C35" t="inlineStr">
         <is>
-          <t>iip_heat_proc</t>
+          <t>sec_heat_high</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="C36" t="inlineStr">
         <is>
-          <t>iip_steel_crudesteel</t>
+          <t>emi_CO2_f_x2x</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="C37" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="C38" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>iip_steel_blafu_slag</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="C39" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>emi_CO2_f_ind</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="C40" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>emi_CH4_f_ind</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="C41" t="inlineStr">
         <is>
-          <t>iip_steel_sponge_iron</t>
+          <t>emi_N2O_f_ind</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="C42" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>exo_steel</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="C43" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>CO2_f_pow</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="C44" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>pri_crude_oil</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="C45" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>[emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="C46" t="inlineStr">
         <is>
-          <t>iip_steel_scrap</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>sec_methane</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>iip_steel_oxygen</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>iip_steel_scrap</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>sec_methane</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_ore</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>iip_steel_oxygen</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>iip_steel_raw_iron</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>sec_methane</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>iip_steel_oxygen</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>iip_steel_raw_iron</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>sec_methane</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>iip_coke</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_ore</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_ore</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>sec_methane</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>pri_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>pri_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_ore</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_ore</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_pellets</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>sec_methane</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>sec_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>sec_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>pri_biomass</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>pri_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>sec_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>pri_waste</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>pri_geoth_heat</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>pri_geoth_heat</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>pri_geoth_heat</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>pri_geoth_heat</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>pri_hydro_energy</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>pri_hydro_energy</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>pri_hydro_energy</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>pri_uran</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>pri_deuterium</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>pri_solar_radiation</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>pri_solar_radiation</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>pri_solar_radiation</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>pri_wind_energy_off</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>pri_wind_energy_off</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>pri_wind_energy_on</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>sec_heat_low</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>sec_heat_high</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>sec_heat_high</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>sec_heat_low</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>sec_heat_low</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>sec_heat_high</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>sec_heat_high</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>sec_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>sec_heat_high</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>sec_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>sec_heat_high</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>sec_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>iip_coke</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_ore</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>iip_steel_oxygen</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>iip_steel_scrap</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>iip_steel_raw_iron</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>iip_steel_blafu_slag</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>iip_steel_raw_iron</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>iip_steel_blafu_slag</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>iip_steel_raw_iron</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>iip_steel_blafu_slag</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>iip_heat_proc</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>exo_steel</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>exo_steel</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>iip_steel_crudesteel</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>iip_steel_crudesteel</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="185">
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>iip_steel_crudesteel</t>
-        </is>
-      </c>
-    </row>
-    <row r="186">
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="187">
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="C189" t="inlineStr">
-        <is>
-          <t>iip_steel_crudesteel</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>iip_steel_crudesteel</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="192">
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="193">
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="194">
-      <c r="C194" t="inlineStr">
-        <is>
-          <t>iip_steel_crudesteel</t>
-        </is>
-      </c>
-    </row>
-    <row r="195">
-      <c r="C195" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="196">
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_pellets</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="202">
-      <c r="C202" t="inlineStr">
-        <is>
-          <t>iip_steel_sinter</t>
-        </is>
-      </c>
-    </row>
-    <row r="203">
-      <c r="C203" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="204">
-      <c r="C204" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="205">
-      <c r="C205" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="206">
-      <c r="C206" t="inlineStr">
-        <is>
-          <t>iip_steel_sinter</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="C207" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="C209" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="210">
-      <c r="C210" t="inlineStr">
-        <is>
-          <t>iip_steel_sponge_iron</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="C211" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="212">
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="213">
-      <c r="C213" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="214">
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="215">
-      <c r="C215" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="216">
-      <c r="C216" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="217">
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="218">
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="219">
-      <c r="C219" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="220">
-      <c r="C220" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="221">
-      <c r="C221" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="222">
-      <c r="C222" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="223">
-      <c r="C223" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="224">
-      <c r="C224" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="225">
-      <c r="C225" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="226">
-      <c r="C226" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="227">
-      <c r="C227" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="228">
-      <c r="C228" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="229">
-      <c r="C229" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="230">
-      <c r="C230" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="231">
-      <c r="C231" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="232">
-      <c r="C232" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="233">
-      <c r="C233" t="inlineStr">
-        <is>
-          <t>sec_heat_low</t>
-        </is>
-      </c>
-    </row>
-    <row r="234">
-      <c r="C234" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="235">
-      <c r="C235" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="236">
-      <c r="C236" t="inlineStr">
-        <is>
-          <t>sec_heat_low</t>
-        </is>
-      </c>
-    </row>
-    <row r="237">
-      <c r="C237" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="238">
-      <c r="C238" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="239">
-      <c r="C239" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="240">
-      <c r="C240" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="241">
-      <c r="C241" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="242">
-      <c r="C242" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="243">
-      <c r="C243" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="244">
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="245">
-      <c r="C245" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="246">
-      <c r="C246" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="247">
-      <c r="C247" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="248">
-      <c r="C248" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="249">
-      <c r="C249" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="250">
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="251">
-      <c r="C251" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="252">
-      <c r="C252" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="253">
-      <c r="C253" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="254">
-      <c r="C254" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="255">
-      <c r="C255" t="inlineStr">
-        <is>
-          <t>sec_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="256">
-      <c r="C256" t="inlineStr">
-        <is>
-          <t>pri_biomass</t>
-        </is>
-      </c>
-    </row>
-    <row r="257">
-      <c r="C257" t="inlineStr">
-        <is>
-          <t>pri_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="258">
-      <c r="C258" t="inlineStr">
-        <is>
-          <t>pri_crude_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="259">
-      <c r="C259" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="260">
-      <c r="C260" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="261">
-      <c r="C261" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="262">
-      <c r="C262" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="263">
-      <c r="C263" t="inlineStr">
-        <is>
-          <t>[emi_CO2_f_x2x_neg_reusable</t>
-        </is>
-      </c>
-    </row>
-    <row r="264">
-      <c r="C264" t="inlineStr">
-        <is>
           <t>emi_CO2_f_x2x_neg_stored]</t>
-        </is>
-      </c>
-    </row>
-    <row r="265">
-      <c r="C265" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="266">
-      <c r="C266" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="267">
-      <c r="C267" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="268">
-      <c r="C268" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="269">
-      <c r="C269" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="270">
-      <c r="C270" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="271">
-      <c r="C271" t="inlineStr">
-        <is>
-          <t>sec_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="272">
-      <c r="C272" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="273">
-      <c r="C273" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="274">
-      <c r="C274" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="275">
-      <c r="C275" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="276">
-      <c r="C276" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="277">
-      <c r="C277" t="inlineStr">
-        <is>
-          <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="278">
-      <c r="C278" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x</t>
         </is>
       </c>
     </row>
@@ -11595,7 +9965,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I278"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11743,1888 +10113,481 @@
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_blafu_1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_blafu_ccs_1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_boiler_0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_casting_0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_casting_1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_dirred_1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="C15" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_elefu_0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="C16" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_elefu_1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_hyddri_1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="C18" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_oxyfu_0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="C19" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_oxyfu_1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_0</t>
+          <t>ind_steel_pellet_1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="C21" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>ind_steel_sinter_0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="C22" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>ind_steel_sinter_1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="C23" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>ind_steel_sponge_1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="C24" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_gt_biogas</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="C25" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_gt_heating_oil</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="C26" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_gt_hydrogen</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="C27" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_gt_natgas</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_gt_sng</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="C29" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_st_biomass</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="C30" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_st_coal</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="C31" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_st_heating_oil</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="C32" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_st_natgas</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="C33" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_1</t>
+          <t>pow_combustion_st_waste</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="C34" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_geothermal_orc</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="C35" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_geothermal_orc_chp</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="C36" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_geothermal_st</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="C37" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_geothermal_st_chp</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="C38" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_hydro_pond</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="C39" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_hydro_ror</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="C40" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_hydro_ror_pond</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="C41" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_nuclear_fis</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="C42" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_nuclear_fus</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="C43" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_photovoltaic_cts_roof</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="C44" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_photovoltaic_fiel_gm</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="C45" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_photovoltaic_hh_roof</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="C46" t="inlineStr">
         <is>
-          <t>ind_steel_blafu_ccs_1</t>
+          <t>pow_storage_cts</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="C47" t="inlineStr">
         <is>
-          <t>ind_steel_boiler_0</t>
+          <t>pow_storage_hh</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="C48" t="inlineStr">
         <is>
-          <t>ind_steel_boiler_0</t>
+          <t>pow_storage_hydr</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="C49" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>pow_storage_ind</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="C50" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>pow_storage_util</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="C51" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>pow_wind-turbine_off_fb</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="C52" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>pow_wind-turbine_off_fl</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="C53" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>pow_wind-turbine_on</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="C54" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>x2x_g2p_pemfc_ls</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="C55" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>x2x_g2p_sofc_ls</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="C56" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>x2x_import_biogas</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="C57" t="inlineStr">
         <is>
-          <t>ind_steel_casting_0</t>
+          <t>x2x_import_biomass</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="C58" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_import_coal</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="C59" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_import_crudeoil</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="C60" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_import_elec</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="C61" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_import_h2</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="C62" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_import_natural_gas</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="C63" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_import_sng</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="C64" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_other_daccs</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="C65" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_p2gas_aec</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="C66" t="inlineStr">
         <is>
-          <t>ind_steel_casting_1</t>
+          <t>x2x_p2gas_bioem</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="C67" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_p2gas_biom</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="C68" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_p2gas_pemec</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="C69" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_p2gas_sabm</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="C70" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_p2gas_soec</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="C71" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_storage_ch4_biogas</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="C72" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_storage_ch4_natural_gas</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="C73" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_storage_ch4_sng</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="C74" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_storage_h2</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="C75" t="inlineStr">
         <is>
-          <t>ind_steel_dirred_1</t>
+          <t>x2x_storage_h2_lohc</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="C76" t="inlineStr">
         <is>
-          <t>ind_steel_elefu_0</t>
+          <t>x2x_x2gas_mpyr</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="C77" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>ind_steel_elefu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>ind_steel_hyddri_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>ind_steel_hyddri_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>ind_steel_hyddri_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>ind_steel_hyddri_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>ind_steel_oxyfu_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>ind_steel_pellet_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>ind_steel_pellet_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>ind_steel_pellet_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>ind_steel_pellet_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>ind_steel_pellet_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>ind_steel_pellet_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>ind_steel_pellet_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_0</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>ind_steel_sinter_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>ind_steel_sponge_1</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_natgas</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_natgas</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_natgas</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_sng</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_sng</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>pow_combustion_gt_sng</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_biomass</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_biomass</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_natgas</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_natgas</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_natgas</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_waste</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_waste</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>pow_combustion_st_waste</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>pow_geothermal_orc</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>pow_geothermal_orc</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>pow_geothermal_orc_chp</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>pow_geothermal_orc_chp</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>pow_geothermal_orc_chp</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>pow_geothermal_st</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>pow_geothermal_st</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>pow_geothermal_st_chp</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>pow_geothermal_st_chp</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>pow_geothermal_st_chp</t>
-        </is>
-      </c>
-    </row>
-    <row r="185">
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>pow_hydro_pond</t>
-        </is>
-      </c>
-    </row>
-    <row r="186">
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>pow_hydro_pond</t>
-        </is>
-      </c>
-    </row>
-    <row r="187">
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>pow_hydro_ror</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>pow_hydro_ror</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="C189" t="inlineStr">
-        <is>
-          <t>pow_hydro_ror_pond</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>pow_hydro_ror_pond</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>pow_nuclear_fis</t>
-        </is>
-      </c>
-    </row>
-    <row r="192">
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>pow_nuclear_fis</t>
-        </is>
-      </c>
-    </row>
-    <row r="193">
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>pow_nuclear_fus</t>
-        </is>
-      </c>
-    </row>
-    <row r="194">
-      <c r="C194" t="inlineStr">
-        <is>
-          <t>pow_nuclear_fus</t>
-        </is>
-      </c>
-    </row>
-    <row r="195">
-      <c r="C195" t="inlineStr">
-        <is>
-          <t>pow_photovoltaic_cts_roof</t>
-        </is>
-      </c>
-    </row>
-    <row r="196">
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>pow_photovoltaic_cts_roof</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>pow_photovoltaic_fiel_gm</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>pow_photovoltaic_fiel_gm</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>pow_photovoltaic_hh_roof</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>pow_photovoltaic_hh_roof</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>pow_storage_cts</t>
-        </is>
-      </c>
-    </row>
-    <row r="202">
-      <c r="C202" t="inlineStr">
-        <is>
-          <t>pow_storage_cts</t>
-        </is>
-      </c>
-    </row>
-    <row r="203">
-      <c r="C203" t="inlineStr">
-        <is>
-          <t>pow_storage_hh</t>
-        </is>
-      </c>
-    </row>
-    <row r="204">
-      <c r="C204" t="inlineStr">
-        <is>
-          <t>pow_storage_hh</t>
-        </is>
-      </c>
-    </row>
-    <row r="205">
-      <c r="C205" t="inlineStr">
-        <is>
-          <t>pow_storage_hydr</t>
-        </is>
-      </c>
-    </row>
-    <row r="206">
-      <c r="C206" t="inlineStr">
-        <is>
-          <t>pow_storage_hydr</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="C207" t="inlineStr">
-        <is>
-          <t>pow_storage_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>pow_storage_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="C209" t="inlineStr">
-        <is>
-          <t>pow_storage_util</t>
-        </is>
-      </c>
-    </row>
-    <row r="210">
-      <c r="C210" t="inlineStr">
-        <is>
-          <t>pow_storage_util</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="C211" t="inlineStr">
-        <is>
-          <t>pow_wind-turbine_off_fb</t>
-        </is>
-      </c>
-    </row>
-    <row r="212">
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>pow_wind-turbine_off_fb</t>
-        </is>
-      </c>
-    </row>
-    <row r="213">
-      <c r="C213" t="inlineStr">
-        <is>
-          <t>pow_wind-turbine_off_fl</t>
-        </is>
-      </c>
-    </row>
-    <row r="214">
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>pow_wind-turbine_off_fl</t>
-        </is>
-      </c>
-    </row>
-    <row r="215">
-      <c r="C215" t="inlineStr">
-        <is>
-          <t>pow_wind-turbine_on</t>
-        </is>
-      </c>
-    </row>
-    <row r="216">
-      <c r="C216" t="inlineStr">
-        <is>
-          <t>pow_wind-turbine_on</t>
-        </is>
-      </c>
-    </row>
-    <row r="217">
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>x2x_g2p_pemfc_ls</t>
-        </is>
-      </c>
-    </row>
-    <row r="218">
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>x2x_g2p_pemfc_ls</t>
-        </is>
-      </c>
-    </row>
-    <row r="219">
-      <c r="C219" t="inlineStr">
-        <is>
-          <t>x2x_g2p_pemfc_ls</t>
-        </is>
-      </c>
-    </row>
-    <row r="220">
-      <c r="C220" t="inlineStr">
-        <is>
-          <t>x2x_g2p_sofc_ls</t>
-        </is>
-      </c>
-    </row>
-    <row r="221">
-      <c r="C221" t="inlineStr">
-        <is>
-          <t>x2x_g2p_sofc_ls</t>
-        </is>
-      </c>
-    </row>
-    <row r="222">
-      <c r="C222" t="inlineStr">
-        <is>
-          <t>x2x_g2p_sofc_ls</t>
-        </is>
-      </c>
-    </row>
-    <row r="223">
-      <c r="C223" t="inlineStr">
-        <is>
-          <t>x2x_import_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="224">
-      <c r="C224" t="inlineStr">
-        <is>
-          <t>x2x_import_biomass</t>
-        </is>
-      </c>
-    </row>
-    <row r="225">
-      <c r="C225" t="inlineStr">
-        <is>
-          <t>x2x_import_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="226">
-      <c r="C226" t="inlineStr">
-        <is>
-          <t>x2x_import_crudeoil</t>
-        </is>
-      </c>
-    </row>
-    <row r="227">
-      <c r="C227" t="inlineStr">
-        <is>
-          <t>x2x_import_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="228">
-      <c r="C228" t="inlineStr">
-        <is>
-          <t>x2x_import_h2</t>
-        </is>
-      </c>
-    </row>
-    <row r="229">
-      <c r="C229" t="inlineStr">
-        <is>
-          <t>x2x_import_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="230">
-      <c r="C230" t="inlineStr">
-        <is>
-          <t>x2x_import_sng</t>
-        </is>
-      </c>
-    </row>
-    <row r="231">
-      <c r="C231" t="inlineStr">
-        <is>
-          <t>x2x_other_daccs</t>
-        </is>
-      </c>
-    </row>
-    <row r="232">
-      <c r="C232" t="inlineStr">
-        <is>
-          <t>x2x_other_daccs</t>
-        </is>
-      </c>
-    </row>
-    <row r="233">
-      <c r="C233" t="inlineStr">
-        <is>
-          <t>x2x_other_daccs</t>
-        </is>
-      </c>
-    </row>
-    <row r="234">
-      <c r="C234" t="inlineStr">
-        <is>
-          <t>x2x_other_daccs</t>
-        </is>
-      </c>
-    </row>
-    <row r="235">
-      <c r="C235" t="inlineStr">
-        <is>
-          <t>x2x_other_daccs</t>
-        </is>
-      </c>
-    </row>
-    <row r="236">
-      <c r="C236" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_aec</t>
-        </is>
-      </c>
-    </row>
-    <row r="237">
-      <c r="C237" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_aec</t>
-        </is>
-      </c>
-    </row>
-    <row r="238">
-      <c r="C238" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_aec</t>
-        </is>
-      </c>
-    </row>
-    <row r="239">
-      <c r="C239" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_bioem</t>
-        </is>
-      </c>
-    </row>
-    <row r="240">
-      <c r="C240" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_bioem</t>
-        </is>
-      </c>
-    </row>
-    <row r="241">
-      <c r="C241" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_bioem</t>
-        </is>
-      </c>
-    </row>
-    <row r="242">
-      <c r="C242" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_bioem</t>
-        </is>
-      </c>
-    </row>
-    <row r="243">
-      <c r="C243" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_biom</t>
-        </is>
-      </c>
-    </row>
-    <row r="244">
-      <c r="C244" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_biom</t>
-        </is>
-      </c>
-    </row>
-    <row r="245">
-      <c r="C245" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_biom</t>
-        </is>
-      </c>
-    </row>
-    <row r="246">
-      <c r="C246" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_biom</t>
-        </is>
-      </c>
-    </row>
-    <row r="247">
-      <c r="C247" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_pemec</t>
-        </is>
-      </c>
-    </row>
-    <row r="248">
-      <c r="C248" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_pemec</t>
-        </is>
-      </c>
-    </row>
-    <row r="249">
-      <c r="C249" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_pemec</t>
-        </is>
-      </c>
-    </row>
-    <row r="250">
-      <c r="C250" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_sabm</t>
-        </is>
-      </c>
-    </row>
-    <row r="251">
-      <c r="C251" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_sabm</t>
-        </is>
-      </c>
-    </row>
-    <row r="252">
-      <c r="C252" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_sabm</t>
-        </is>
-      </c>
-    </row>
-    <row r="253">
-      <c r="C253" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_sabm</t>
-        </is>
-      </c>
-    </row>
-    <row r="254">
-      <c r="C254" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_sabm</t>
-        </is>
-      </c>
-    </row>
-    <row r="255">
-      <c r="C255" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_soec</t>
-        </is>
-      </c>
-    </row>
-    <row r="256">
-      <c r="C256" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_soec</t>
-        </is>
-      </c>
-    </row>
-    <row r="257">
-      <c r="C257" t="inlineStr">
-        <is>
-          <t>x2x_p2gas_soec</t>
-        </is>
-      </c>
-    </row>
-    <row r="258">
-      <c r="C258" t="inlineStr">
-        <is>
-          <t>x2x_storage_ch4_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="259">
-      <c r="C259" t="inlineStr">
-        <is>
-          <t>x2x_storage_ch4_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="260">
-      <c r="C260" t="inlineStr">
-        <is>
-          <t>x2x_storage_ch4_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="261">
-      <c r="C261" t="inlineStr">
-        <is>
-          <t>x2x_storage_ch4_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="262">
-      <c r="C262" t="inlineStr">
-        <is>
-          <t>x2x_storage_ch4_sng</t>
-        </is>
-      </c>
-    </row>
-    <row r="263">
-      <c r="C263" t="inlineStr">
-        <is>
-          <t>x2x_storage_ch4_sng</t>
-        </is>
-      </c>
-    </row>
-    <row r="264">
-      <c r="C264" t="inlineStr">
-        <is>
-          <t>x2x_storage_h2</t>
-        </is>
-      </c>
-    </row>
-    <row r="265">
-      <c r="C265" t="inlineStr">
-        <is>
-          <t>x2x_storage_h2</t>
-        </is>
-      </c>
-    </row>
-    <row r="266">
-      <c r="C266" t="inlineStr">
-        <is>
-          <t>x2x_storage_h2_lohc</t>
-        </is>
-      </c>
-    </row>
-    <row r="267">
-      <c r="C267" t="inlineStr">
-        <is>
-          <t>x2x_storage_h2_lohc</t>
-        </is>
-      </c>
-    </row>
-    <row r="268">
-      <c r="C268" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_mpyr</t>
-        </is>
-      </c>
-    </row>
-    <row r="269">
-      <c r="C269" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_mpyr</t>
-        </is>
-      </c>
-    </row>
-    <row r="270">
-      <c r="C270" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_mpyr</t>
-        </is>
-      </c>
-    </row>
-    <row r="271">
-      <c r="C271" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_mpyr</t>
-        </is>
-      </c>
-    </row>
-    <row r="272">
-      <c r="C272" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_mpyr</t>
-        </is>
-      </c>
-    </row>
-    <row r="273">
-      <c r="C273" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_sr</t>
-        </is>
-      </c>
-    </row>
-    <row r="274">
-      <c r="C274" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_sr</t>
-        </is>
-      </c>
-    </row>
-    <row r="275">
-      <c r="C275" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_sr</t>
-        </is>
-      </c>
-    </row>
-    <row r="276">
-      <c r="C276" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_sr</t>
-        </is>
-      </c>
-    </row>
-    <row r="277">
-      <c r="C277" t="inlineStr">
-        <is>
-          <t>x2x_x2gas_sr</t>
-        </is>
-      </c>
-    </row>
-    <row r="278">
-      <c r="C278" t="inlineStr">
         <is>
           <t>x2x_x2gas_sr</t>
         </is>

</xml_diff>

<commit_message>
added cset and pset logic with mapping xlsx
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -9654,303 +9654,518 @@
       </c>
     </row>
     <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>sec_biogas</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>emi_CO2_f_ind</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>emi_CO2_f_x2x_neg_reusable</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>pri_uran</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>emi_N2O_f_ind</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>iip_steel_oxygen</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>iip_steel_iron_pellets</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>exo_steel</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>pri_deuterium</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>pri_coal</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>iip_steel_blafu_slag</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>pri_crude_oil</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>pri_hydro_energy</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sec_methane</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sec_heating_oil</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sec_hydrogen</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sec_heat_low</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>iip_heat_proc</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>sec_elec_ind</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pri_coal</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>pri_biomass</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>pri_waste</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CO2_f_pow</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>emi_CO2_f_x2x_neg_stored]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
         <is>
           <t>iip_coke</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>pri_solar_radiation</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="C8" t="inlineStr">
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>emi_CH4_f_ind</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>iip_steel_raw_iron</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>iip_steel_crudesteel</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>pri_geoth_heat</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>pri_wind_energy_on</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>iip_steel_scrap</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>sec_elec</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>sec_natural_gas_syn</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>[emi_CO2_f_x2x_neg_reusable</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>iip_steel_iron_ore</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>pri_natural_gas</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>pri_wind_energy_off</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
         <is>
           <t>iip_steel_sinter</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>iip_steel_oxygen</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>sec_methane</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>sec_hydrogen</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>iip_heat_proc</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>iip_steel_crudesteel</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" t="inlineStr">
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>MAT</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
         <is>
           <t>iip_steel_sponge_iron</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>iip_steel_scrap</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_ore</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>iip_steel_raw_iron</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>iip_steel_iron_pellets</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>sec_biogas</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>sec_heating_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="C21" t="inlineStr">
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>sec_heat_high</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ENV</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>emi_CO2_f_x2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
         <is>
           <t>sec_H2</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>pri_natural_gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>sec_natural_gas_syn</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>pri_biomass</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>pri_waste</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>pri_geoth_heat</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>pri_hydro_energy</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>pri_uran</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>pri_deuterium</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>pri_solar_radiation</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>sec_elec</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>pri_wind_energy_off</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>pri_wind_energy_on</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>sec_heat_low</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>sec_heat_high</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>iip_steel_blafu_slag</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>emi_CH4_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>emi_N2O_f_ind</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>exo_steel</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>CO2_f_pow</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>pri_crude_oil</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>[emi_CO2_f_x2x_neg_reusable</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>emi_CO2_f_x2x_neg_stored]</t>
         </is>
       </c>
     </row>
@@ -10076,6 +10291,11 @@
       </c>
     </row>
     <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>ind_source_steel_coke</t>
@@ -10083,6 +10303,11 @@
       </c>
     </row>
     <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>ind_source_steel_iron_ore</t>
@@ -10090,6 +10315,11 @@
       </c>
     </row>
     <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>ind_source_steel_oxygen</t>
@@ -10097,6 +10327,11 @@
       </c>
     </row>
     <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>ind_source_steel_scrap_iron</t>
@@ -10104,6 +10339,11 @@
       </c>
     </row>
     <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>ind_steel_blafu_0</t>
@@ -10111,6 +10351,11 @@
       </c>
     </row>
     <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>ind_steel_blafu_1</t>
@@ -10118,6 +10363,11 @@
       </c>
     </row>
     <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>ind_steel_blafu_ccs_1</t>
@@ -10125,6 +10375,11 @@
       </c>
     </row>
     <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>ind_steel_boiler_0</t>
@@ -10132,6 +10387,11 @@
       </c>
     </row>
     <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>ind_steel_casting_0</t>
@@ -10139,6 +10399,11 @@
       </c>
     </row>
     <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>ind_steel_casting_1</t>
@@ -10146,6 +10411,11 @@
       </c>
     </row>
     <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>ind_steel_dirred_1</t>
@@ -10153,6 +10423,11 @@
       </c>
     </row>
     <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>ind_steel_elefu_0</t>
@@ -10160,6 +10435,11 @@
       </c>
     </row>
     <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>ind_steel_elefu_1</t>
@@ -10167,6 +10447,11 @@
       </c>
     </row>
     <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>ind_steel_hyddri_1</t>
@@ -10174,6 +10459,11 @@
       </c>
     </row>
     <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>ind_steel_oxyfu_0</t>
@@ -10181,6 +10471,11 @@
       </c>
     </row>
     <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>ind_steel_oxyfu_1</t>
@@ -10188,6 +10483,11 @@
       </c>
     </row>
     <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>ind_steel_pellet_1</t>
@@ -10195,6 +10495,11 @@
       </c>
     </row>
     <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>ind_steel_sinter_0</t>
@@ -10202,6 +10507,11 @@
       </c>
     </row>
     <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>ind_steel_sinter_1</t>
@@ -10209,6 +10519,11 @@
       </c>
     </row>
     <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>ind_steel_sponge_1</t>
@@ -10216,6 +10531,11 @@
       </c>
     </row>
     <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>pow_combustion_gt_biogas</t>
@@ -10223,6 +10543,11 @@
       </c>
     </row>
     <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>pow_combustion_gt_heating_oil</t>
@@ -10230,6 +10555,11 @@
       </c>
     </row>
     <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>pow_combustion_gt_hydrogen</t>
@@ -10237,6 +10567,11 @@
       </c>
     </row>
     <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>pow_combustion_gt_natgas</t>
@@ -10244,6 +10579,11 @@
       </c>
     </row>
     <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>pow_combustion_gt_sng</t>
@@ -10251,6 +10591,11 @@
       </c>
     </row>
     <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>pow_combustion_st_biomass</t>
@@ -10258,6 +10603,11 @@
       </c>
     </row>
     <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>pow_combustion_st_coal</t>
@@ -10265,6 +10615,11 @@
       </c>
     </row>
     <row r="31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>pow_combustion_st_heating_oil</t>
@@ -10272,6 +10627,11 @@
       </c>
     </row>
     <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>pow_combustion_st_natgas</t>
@@ -10279,6 +10639,11 @@
       </c>
     </row>
     <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>pow_combustion_st_waste</t>
@@ -10286,6 +10651,11 @@
       </c>
     </row>
     <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>pow_geothermal_orc</t>
@@ -10293,6 +10663,11 @@
       </c>
     </row>
     <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CHP</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>pow_geothermal_orc_chp</t>
@@ -10300,6 +10675,11 @@
       </c>
     </row>
     <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>pow_geothermal_st</t>
@@ -10307,6 +10687,11 @@
       </c>
     </row>
     <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CHP</t>
+        </is>
+      </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>pow_geothermal_st_chp</t>
@@ -10314,6 +10699,11 @@
       </c>
     </row>
     <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C38" t="inlineStr">
         <is>
           <t>pow_hydro_pond</t>
@@ -10321,6 +10711,11 @@
       </c>
     </row>
     <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>pow_hydro_ror</t>
@@ -10328,6 +10723,11 @@
       </c>
     </row>
     <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C40" t="inlineStr">
         <is>
           <t>pow_hydro_ror_pond</t>
@@ -10335,6 +10735,11 @@
       </c>
     </row>
     <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>pow_nuclear_fis</t>
@@ -10342,6 +10747,11 @@
       </c>
     </row>
     <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>pow_nuclear_fus</t>
@@ -10349,6 +10759,11 @@
       </c>
     </row>
     <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>pow_photovoltaic_cts_roof</t>
@@ -10356,6 +10771,11 @@
       </c>
     </row>
     <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C44" t="inlineStr">
         <is>
           <t>pow_photovoltaic_fiel_gm</t>
@@ -10363,6 +10783,11 @@
       </c>
     </row>
     <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C45" t="inlineStr">
         <is>
           <t>pow_photovoltaic_hh_roof</t>
@@ -10370,6 +10795,11 @@
       </c>
     </row>
     <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>pow_storage_cts</t>
@@ -10377,6 +10807,11 @@
       </c>
     </row>
     <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>pow_storage_hh</t>
@@ -10384,6 +10819,11 @@
       </c>
     </row>
     <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>pow_storage_hydr</t>
@@ -10391,6 +10831,11 @@
       </c>
     </row>
     <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C49" t="inlineStr">
         <is>
           <t>pow_storage_ind</t>
@@ -10398,6 +10843,11 @@
       </c>
     </row>
     <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>pow_storage_util</t>
@@ -10405,6 +10855,11 @@
       </c>
     </row>
     <row r="51">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>pow_wind-turbine_off_fb</t>
@@ -10412,6 +10867,11 @@
       </c>
     </row>
     <row r="52">
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>pow_wind-turbine_off_fl</t>
@@ -10419,6 +10879,11 @@
       </c>
     </row>
     <row r="53">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>pow_wind-turbine_on</t>
@@ -10426,6 +10891,11 @@
       </c>
     </row>
     <row r="54">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>x2x_g2p_pemfc_ls</t>
@@ -10433,6 +10903,11 @@
       </c>
     </row>
     <row r="55">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>x2x_g2p_sofc_ls</t>
@@ -10440,6 +10915,11 @@
       </c>
     </row>
     <row r="56">
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>x2x_import_biogas</t>
@@ -10447,6 +10927,11 @@
       </c>
     </row>
     <row r="57">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>x2x_import_biomass</t>
@@ -10454,6 +10939,11 @@
       </c>
     </row>
     <row r="58">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>x2x_import_coal</t>
@@ -10461,6 +10951,11 @@
       </c>
     </row>
     <row r="59">
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>x2x_import_crudeoil</t>
@@ -10468,6 +10963,11 @@
       </c>
     </row>
     <row r="60">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>x2x_import_elec</t>
@@ -10475,6 +10975,11 @@
       </c>
     </row>
     <row r="61">
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C61" t="inlineStr">
         <is>
           <t>x2x_import_h2</t>
@@ -10482,6 +10987,11 @@
       </c>
     </row>
     <row r="62">
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>x2x_import_natural_gas</t>
@@ -10489,6 +10999,11 @@
       </c>
     </row>
     <row r="63">
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>x2x_import_sng</t>
@@ -10496,6 +11011,11 @@
       </c>
     </row>
     <row r="64">
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C64" t="inlineStr">
         <is>
           <t>x2x_other_daccs</t>
@@ -10503,6 +11023,11 @@
       </c>
     </row>
     <row r="65">
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>x2x_p2gas_aec</t>
@@ -10510,6 +11035,11 @@
       </c>
     </row>
     <row r="66">
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>x2x_p2gas_bioem</t>
@@ -10517,6 +11047,11 @@
       </c>
     </row>
     <row r="67">
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>x2x_p2gas_biom</t>
@@ -10524,6 +11059,11 @@
       </c>
     </row>
     <row r="68">
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>x2x_p2gas_pemec</t>
@@ -10531,6 +11071,11 @@
       </c>
     </row>
     <row r="69">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>x2x_p2gas_sabm</t>
@@ -10538,6 +11083,11 @@
       </c>
     </row>
     <row r="70">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>x2x_p2gas_soec</t>
@@ -10545,6 +11095,11 @@
       </c>
     </row>
     <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>x2x_storage_ch4_biogas</t>
@@ -10552,6 +11107,11 @@
       </c>
     </row>
     <row r="72">
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>x2x_storage_ch4_natural_gas</t>
@@ -10559,6 +11119,11 @@
       </c>
     </row>
     <row r="73">
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C73" t="inlineStr">
         <is>
           <t>x2x_storage_ch4_sng</t>
@@ -10566,6 +11131,11 @@
       </c>
     </row>
     <row r="74">
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C74" t="inlineStr">
         <is>
           <t>x2x_storage_h2</t>
@@ -10573,6 +11143,11 @@
       </c>
     </row>
     <row r="75">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>x2x_storage_h2_lohc</t>
@@ -10580,6 +11155,11 @@
       </c>
     </row>
     <row r="76">
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C76" t="inlineStr">
         <is>
           <t>x2x_x2gas_mpyr</t>
@@ -10587,6 +11167,11 @@
       </c>
     </row>
     <row r="77">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>PRE</t>
+        </is>
+      </c>
       <c r="C77" t="inlineStr">
         <is>
           <t>x2x_x2gas_sr</t>

</xml_diff>

<commit_message>
add SysSettings and comm grp list
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -10233,7 +10233,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sec_H2</t>
+          <t>pri_wind_energy_on</t>
         </is>
       </c>
     </row>
@@ -10245,31 +10245,31 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>iip_steel_raw_iron</t>
+          <t>iip_steel_crudesteel</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
+          <t>pri_coal</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>sec_heating_oil</t>
+          <t>iip_steel_oxygen</t>
         </is>
       </c>
     </row>
@@ -10281,19 +10281,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>pri_natural_gas</t>
+          <t>sec_H2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[emi_CO2_f_x2x_neg_reusable</t>
+          <t>pri_solar_radiation</t>
         </is>
       </c>
     </row>
@@ -10305,7 +10305,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>pri_waste</t>
+          <t>sec_natural_gas_syn</t>
         </is>
       </c>
     </row>
@@ -10317,67 +10317,67 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sec_heat_high</t>
+          <t>iip_steel_blafu_slag</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>DEM</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>sec_natural_gas_syn</t>
+          <t>exo_steel</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>emi_N2O_f_ind</t>
+          <t>CO2_f_pow</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>iip_steel_sinter</t>
+          <t>emi_CO2_f_x2x_neg_stored]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>iip_steel_iron_pellets</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>iip_steel_scrap</t>
+          <t>pri_crude_oil</t>
         </is>
       </c>
     </row>
@@ -10389,7 +10389,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>iip_steel_blafu_slag</t>
+          <t>sec_heat_high</t>
         </is>
       </c>
     </row>
@@ -10401,7 +10401,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>emi_CH4_f_ind</t>
+          <t>emi_N2O_f_ind</t>
         </is>
       </c>
     </row>
@@ -10413,31 +10413,31 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>sec_biogas</t>
+          <t>iip_coke</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>pri_uran</t>
+          <t>emi_CO2_f_x2x</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x</t>
+          <t>pri_deuterium</t>
         </is>
       </c>
     </row>
@@ -10449,19 +10449,19 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>pri_hydro_energy</t>
+          <t>sec_elec</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>pri_geoth_heat</t>
+          <t>emi_CH4_f_ind</t>
         </is>
       </c>
     </row>
@@ -10473,19 +10473,19 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>pri_coal</t>
+          <t>sec_hydrogen</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>emi_CO2_f_ind</t>
+          <t>iip_steel_iron_ore</t>
         </is>
       </c>
     </row>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>iip_steel_iron_ore</t>
+          <t>iip_steel_scrap</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>pri_crude_oil</t>
+          <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
     </row>
@@ -10521,7 +10521,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>pri_solar_radiation</t>
+          <t>sec_heat_low</t>
         </is>
       </c>
     </row>
@@ -10545,7 +10545,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>pri_biomass</t>
+          <t>iip_heat_proc</t>
         </is>
       </c>
     </row>
@@ -10557,7 +10557,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>pri_deuterium</t>
+          <t>pri_geoth_heat</t>
         </is>
       </c>
     </row>
@@ -10569,7 +10569,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>pri_wind_energy_on</t>
+          <t>pri_wind_energy_off</t>
         </is>
       </c>
     </row>
@@ -10581,19 +10581,19 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>sec_heavy_fuel_oil</t>
+          <t>pri_uran</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>sec_biogas</t>
         </is>
       </c>
     </row>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>iip_heat_proc</t>
+          <t>pri_natural_gas</t>
         </is>
       </c>
     </row>
@@ -10617,19 +10617,19 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>iip_steel_sponge_iron</t>
+          <t>iip_steel_raw_iron</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>iip_steel_iron_pellets</t>
+          <t>emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
@@ -10641,43 +10641,43 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>sec_heat_low</t>
+          <t>pri_waste</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>emi_CO2_f_ind</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>sec_elec</t>
+          <t>iip_steel_sponge_iron</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>pri_wind_energy_off</t>
+          <t>[emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
@@ -10689,7 +10689,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>iip_coke</t>
+          <t>sec_heating_oil</t>
         </is>
       </c>
     </row>
@@ -10701,43 +10701,43 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CO2_f_pow</t>
+          <t>pri_biomass</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>DEM</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>exo_steel</t>
+          <t>iip_steel_sinter</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_stored]</t>
+          <t>sec_elec_ind</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>iip_steel_crudesteel</t>
+          <t>pri_hydro_energy</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified app and get_data for ease during data input
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -10233,19 +10233,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>pri_wind_energy_on</t>
+          <t>iip_heat_proc</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>iip_steel_crudesteel</t>
+          <t>pri_wind_energy_on</t>
         </is>
       </c>
     </row>
@@ -10257,31 +10257,31 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>pri_coal</t>
+          <t>sec_biogas</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>sec_elec</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>sec_H2</t>
+          <t>iip_steel_iron_pellets</t>
         </is>
       </c>
     </row>
@@ -10293,19 +10293,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>pri_solar_radiation</t>
+          <t>sec_heat_low</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>sec_natural_gas_syn</t>
+          <t>emi_CH4_f_ind</t>
         </is>
       </c>
     </row>
@@ -10317,19 +10317,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>iip_steel_blafu_slag</t>
+          <t>sec_hydrogen</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>DEM</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>exo_steel</t>
+          <t>emi_N2O_f_ind</t>
         </is>
       </c>
     </row>
@@ -10341,31 +10341,31 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CO2_f_pow</t>
+          <t>sec_H2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_stored]</t>
+          <t>sec_natural_gas_syn</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>iip_steel_iron_pellets</t>
+          <t>iip_steel_blafu_slag</t>
         </is>
       </c>
     </row>
@@ -10377,31 +10377,31 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>pri_crude_oil</t>
+          <t>pri_natural_gas</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>sec_heat_high</t>
+          <t>iip_steel_sinter</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>emi_N2O_f_ind</t>
+          <t>sec_heating_oil</t>
         </is>
       </c>
     </row>
@@ -10413,19 +10413,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>iip_coke</t>
+          <t>sec_elec_ind</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x</t>
+          <t>pri_biomass</t>
         </is>
       </c>
     </row>
@@ -10437,43 +10437,43 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>pri_deuterium</t>
+          <t>pri_wind_energy_off</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>sec_elec</t>
+          <t>iip_steel_scrap</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>emi_CH4_f_ind</t>
+          <t>sec_methane</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>iip_steel_crudesteel</t>
         </is>
       </c>
     </row>
@@ -10485,19 +10485,19 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>iip_steel_iron_ore</t>
+          <t>iip_steel_raw_iron</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>iip_steel_scrap</t>
+          <t>sec_heat_high</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>sec_heavy_fuel_oil</t>
+          <t>pri_hydro_energy</t>
         </is>
       </c>
     </row>
@@ -10521,7 +10521,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>sec_heat_low</t>
+          <t>pri_solar_radiation</t>
         </is>
       </c>
     </row>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>iip_coke</t>
         </is>
       </c>
     </row>
@@ -10545,19 +10545,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>iip_heat_proc</t>
+          <t>pri_crude_oil</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>pri_geoth_heat</t>
+          <t>iip_steel_oxygen</t>
         </is>
       </c>
     </row>
@@ -10569,19 +10569,19 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>pri_wind_energy_off</t>
+          <t>pri_waste</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>pri_uran</t>
+          <t>emi_CO2_f_x2x_neg_stored]</t>
         </is>
       </c>
     </row>
@@ -10593,79 +10593,79 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>sec_biogas</t>
+          <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>pri_natural_gas</t>
+          <t>emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>iip_steel_raw_iron</t>
+          <t>pri_geoth_heat</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
+          <t>iip_steel_iron_ore</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>DEM</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>pri_waste</t>
+          <t>exo_steel</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>emi_CO2_f_ind</t>
+          <t>pri_uran</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>iip_steel_sponge_iron</t>
+          <t>CO2_f_pow</t>
         </is>
       </c>
     </row>
@@ -10684,12 +10684,12 @@
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>sec_heating_oil</t>
+          <t>emi_CO2_f_ind</t>
         </is>
       </c>
     </row>
@@ -10701,7 +10701,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>pri_biomass</t>
+          <t>pri_deuterium</t>
         </is>
       </c>
     </row>
@@ -10713,7 +10713,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>iip_steel_sinter</t>
+          <t>iip_steel_sponge_iron</t>
         </is>
       </c>
     </row>
@@ -10725,19 +10725,19 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>pri_coal</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>pri_hydro_energy</t>
+          <t>emi_CO2_f_x2x</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
retracted back to earlier method to avoid complications
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -10228,36 +10228,36 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>iip_heat_proc</t>
+          <t>iip_steel_oxygen</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>pri_wind_energy_on</t>
+          <t>iip_steel_sinter</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>sec_biogas</t>
+          <t>iip_steel_scrap</t>
         </is>
       </c>
     </row>
@@ -10269,19 +10269,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>sec_elec</t>
+          <t>pri_uran</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>iip_steel_iron_pellets</t>
+          <t>emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
@@ -10293,43 +10293,43 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>sec_heat_low</t>
+          <t>sec_heat_high</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>emi_CH4_f_ind</t>
+          <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>emi_CH4_f_ind</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>emi_N2O_f_ind</t>
+          <t>CO2_f_pow</t>
         </is>
       </c>
     </row>
@@ -10341,67 +10341,67 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>sec_H2</t>
+          <t>pri_biomass</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>sec_natural_gas_syn</t>
+          <t>[emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>iip_steel_blafu_slag</t>
+          <t>emi_CO2_f_ind</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>pri_natural_gas</t>
+          <t>iip_steel_sponge_iron</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>iip_steel_sinter</t>
+          <t>iip_coke</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>sec_heating_oil</t>
+          <t>iip_steel_crudesteel</t>
         </is>
       </c>
     </row>
@@ -10413,7 +10413,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>sec_heat_low</t>
         </is>
       </c>
     </row>
@@ -10425,7 +10425,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>pri_biomass</t>
+          <t>pri_waste</t>
         </is>
       </c>
     </row>
@@ -10444,48 +10444,48 @@
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>iip_steel_scrap</t>
+          <t>pri_crude_oil</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>iip_steel_raw_iron</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>iip_steel_crudesteel</t>
+          <t>sec_biogas</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>iip_steel_raw_iron</t>
+          <t>pri_hydro_energy</t>
         </is>
       </c>
     </row>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>sec_heat_high</t>
+          <t>sec_elec_ind</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>pri_hydro_energy</t>
+          <t>sec_natural_gas_syn</t>
         </is>
       </c>
     </row>
@@ -10521,7 +10521,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>pri_solar_radiation</t>
+          <t>pri_geoth_heat</t>
         </is>
       </c>
     </row>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>iip_coke</t>
+          <t>sec_H2</t>
         </is>
       </c>
     </row>
@@ -10545,7 +10545,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>pri_crude_oil</t>
+          <t>iip_heat_proc</t>
         </is>
       </c>
     </row>
@@ -10557,7 +10557,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>iip_steel_iron_pellets</t>
         </is>
       </c>
     </row>
@@ -10569,79 +10569,79 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>pri_waste</t>
+          <t>sec_elec</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_stored]</t>
+          <t>pri_natural_gas</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>sec_heavy_fuel_oil</t>
+          <t>emi_CO2_f_x2x_neg_stored]</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>DEM</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
+          <t>exo_steel</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>pri_geoth_heat</t>
+          <t>emi_N2O_f_ind</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>iip_steel_iron_ore</t>
+          <t>pri_coal</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>DEM</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>exo_steel</t>
+          <t>sec_heating_oil</t>
         </is>
       </c>
     </row>
@@ -10653,7 +10653,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>pri_uran</t>
+          <t>iip_steel_blafu_slag</t>
         </is>
       </c>
     </row>
@@ -10665,55 +10665,55 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CO2_f_pow</t>
+          <t>pri_solar_radiation</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[emi_CO2_f_x2x_neg_reusable</t>
+          <t>sec_hydrogen</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>emi_CO2_f_ind</t>
+          <t>pri_wind_energy_on</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>pri_deuterium</t>
+          <t>iip_steel_iron_ore</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>iip_steel_sponge_iron</t>
+          <t>sec_methane</t>
         </is>
       </c>
     </row>
@@ -10725,7 +10725,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>pri_coal</t>
+          <t>pri_deuterium</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finished v1 of data mapping
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -511,16 +511,16 @@
     <col width="38" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="11" customWidth="1" min="9" max="9"/>
-    <col width="5" customWidth="1" min="10" max="10"/>
-    <col width="5" customWidth="1" min="11" max="11"/>
-    <col width="5" customWidth="1" min="12" max="12"/>
-    <col width="5" customWidth="1" min="13" max="13"/>
-    <col width="5" customWidth="1" min="14" max="14"/>
-    <col width="5" customWidth="1" min="15" max="15"/>
-    <col width="5" customWidth="1" min="16" max="16"/>
-    <col width="5" customWidth="1" min="17" max="17"/>
-    <col width="5" customWidth="1" min="18" max="18"/>
-    <col width="5" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -744,7 +744,11 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E4" s="7" t="n"/>
+      <c r="E4" s="7" t="inlineStr">
+        <is>
+          <t>sec_elec_ind</t>
+        </is>
+      </c>
       <c r="F4" s="7" t="inlineStr">
         <is>
           <t>iip_coke</t>
@@ -776,7 +780,11 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E5" s="8" t="n"/>
+      <c r="E5" s="8" t="inlineStr">
+        <is>
+          <t>pri_coal</t>
+        </is>
+      </c>
       <c r="F5" s="8" t="inlineStr">
         <is>
           <t>iip_steel_iron_ore</t>
@@ -808,7 +816,11 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E6" s="7" t="n"/>
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>iip_coke</t>
+        </is>
+      </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
           <t>iip_steel_oxygen</t>
@@ -840,7 +852,11 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E7" s="8" t="n"/>
+      <c r="E7" s="8" t="inlineStr">
+        <is>
+          <t>sec_heavy_fuel_oil</t>
+        </is>
+      </c>
       <c r="F7" s="8" t="inlineStr">
         <is>
           <t>iip_steel_scrap</t>
@@ -877,20 +893,40 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F8" s="7" t="n"/>
+      <c r="F8" s="7" t="inlineStr"/>
       <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="7" t="inlineStr"/>
       <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-      <c r="K8" s="7" t="inlineStr"/>
-      <c r="L8" s="7" t="inlineStr"/>
-      <c r="M8" s="7" t="inlineStr"/>
-      <c r="N8" s="7" t="inlineStr"/>
-      <c r="O8" s="7" t="inlineStr"/>
-      <c r="P8" s="7" t="inlineStr"/>
-      <c r="Q8" s="7" t="inlineStr"/>
-      <c r="R8" s="7" t="inlineStr"/>
-      <c r="S8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="K8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="L8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="M8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="N8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="O8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="P8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="Q8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="R8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
+      <c r="S8" s="7" t="n">
+        <v>0.6854</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="7" t="inlineStr">
@@ -909,20 +945,40 @@
           <t>pri_coal</t>
         </is>
       </c>
-      <c r="F9" s="7" t="n"/>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
       <c r="I9" s="7" t="inlineStr"/>
-      <c r="J9" s="7" t="inlineStr"/>
-      <c r="K9" s="7" t="inlineStr"/>
-      <c r="L9" s="7" t="inlineStr"/>
-      <c r="M9" s="7" t="inlineStr"/>
-      <c r="N9" s="7" t="inlineStr"/>
-      <c r="O9" s="7" t="inlineStr"/>
-      <c r="P9" s="7" t="inlineStr"/>
-      <c r="Q9" s="7" t="inlineStr"/>
-      <c r="R9" s="7" t="inlineStr"/>
-      <c r="S9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="M9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="P9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="R9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
+      <c r="S9" s="7" t="n">
+        <v>4.7396</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="7" t="inlineStr">
@@ -941,20 +997,40 @@
           <t>iip_coke</t>
         </is>
       </c>
-      <c r="F10" s="7" t="n"/>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr"/>
-      <c r="K10" s="7" t="inlineStr"/>
-      <c r="L10" s="7" t="inlineStr"/>
-      <c r="M10" s="7" t="inlineStr"/>
-      <c r="N10" s="7" t="inlineStr"/>
-      <c r="O10" s="7" t="inlineStr"/>
-      <c r="P10" s="7" t="inlineStr"/>
-      <c r="Q10" s="7" t="inlineStr"/>
-      <c r="R10" s="7" t="inlineStr"/>
-      <c r="S10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="K10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="M10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="N10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="O10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="P10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="R10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
+      <c r="S10" s="7" t="n">
+        <v>3.1158</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="7" t="inlineStr">
@@ -973,20 +1049,40 @@
           <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
-      <c r="F11" s="7" t="n"/>
+      <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
       <c r="H11" s="7" t="inlineStr"/>
       <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-      <c r="K11" s="7" t="inlineStr"/>
-      <c r="L11" s="7" t="inlineStr"/>
-      <c r="M11" s="7" t="inlineStr"/>
-      <c r="N11" s="7" t="inlineStr"/>
-      <c r="O11" s="7" t="inlineStr"/>
-      <c r="P11" s="7" t="inlineStr"/>
-      <c r="Q11" s="7" t="inlineStr"/>
-      <c r="R11" s="7" t="inlineStr"/>
-      <c r="S11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="K11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="L11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="M11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="N11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="O11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="P11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="Q11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="R11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
+      <c r="S11" s="7" t="n">
+        <v>0.3714</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="7" t="inlineStr">
@@ -1005,20 +1101,40 @@
           <t>iip_steel_sinter</t>
         </is>
       </c>
-      <c r="F12" s="7" t="n"/>
+      <c r="F12" s="7" t="inlineStr"/>
       <c r="G12" s="7" t="inlineStr"/>
       <c r="H12" s="7" t="inlineStr"/>
       <c r="I12" s="7" t="inlineStr"/>
-      <c r="J12" s="7" t="inlineStr"/>
-      <c r="K12" s="7" t="inlineStr"/>
-      <c r="L12" s="7" t="inlineStr"/>
-      <c r="M12" s="7" t="inlineStr"/>
-      <c r="N12" s="7" t="inlineStr"/>
-      <c r="O12" s="7" t="inlineStr"/>
-      <c r="P12" s="7" t="inlineStr"/>
-      <c r="Q12" s="7" t="inlineStr"/>
-      <c r="R12" s="7" t="inlineStr"/>
-      <c r="S12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="K12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="L12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="M12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="N12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="O12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="P12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="Q12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="R12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
+      <c r="S12" s="7" t="n">
+        <v>0.9415</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="7" t="inlineStr">
@@ -1037,7 +1153,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F13" s="7" t="n"/>
+      <c r="F13" s="7" t="inlineStr"/>
       <c r="G13" s="7" t="inlineStr"/>
       <c r="H13" s="7" t="inlineStr"/>
       <c r="I13" s="7" t="inlineStr"/>
@@ -1064,7 +1180,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E14" s="7" t="n"/>
+      <c r="E14" s="7" t="inlineStr"/>
       <c r="F14" s="7" t="inlineStr">
         <is>
           <t>iip_steel_raw_iron</t>
@@ -1073,16 +1189,36 @@
       <c r="G14" s="7" t="inlineStr"/>
       <c r="H14" s="7" t="inlineStr"/>
       <c r="I14" s="7" t="inlineStr"/>
-      <c r="J14" s="7" t="inlineStr"/>
-      <c r="K14" s="7" t="inlineStr"/>
-      <c r="L14" s="7" t="inlineStr"/>
-      <c r="M14" s="7" t="inlineStr"/>
-      <c r="N14" s="7" t="inlineStr"/>
-      <c r="O14" s="7" t="inlineStr"/>
-      <c r="P14" s="7" t="inlineStr"/>
-      <c r="Q14" s="7" t="inlineStr"/>
-      <c r="R14" s="7" t="inlineStr"/>
-      <c r="S14" s="7" t="inlineStr"/>
+      <c r="J14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S14" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="7" t="inlineStr">
@@ -1096,7 +1232,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E15" s="7" t="n"/>
+      <c r="E15" s="7" t="inlineStr"/>
       <c r="F15" s="7" t="inlineStr">
         <is>
           <t>iip_steel_blafu_slag</t>
@@ -1105,16 +1241,36 @@
       <c r="G15" s="7" t="inlineStr"/>
       <c r="H15" s="7" t="inlineStr"/>
       <c r="I15" s="7" t="inlineStr"/>
-      <c r="J15" s="7" t="inlineStr"/>
-      <c r="K15" s="7" t="inlineStr"/>
-      <c r="L15" s="7" t="inlineStr"/>
-      <c r="M15" s="7" t="inlineStr"/>
-      <c r="N15" s="7" t="inlineStr"/>
-      <c r="O15" s="7" t="inlineStr"/>
-      <c r="P15" s="7" t="inlineStr"/>
-      <c r="Q15" s="7" t="inlineStr"/>
-      <c r="R15" s="7" t="inlineStr"/>
-      <c r="S15" s="7" t="inlineStr"/>
+      <c r="J15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="P15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R15" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S15" s="7" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="7" t="inlineStr">
@@ -1128,7 +1284,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E16" s="7" t="n"/>
+      <c r="E16" s="7" t="inlineStr"/>
       <c r="F16" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -1160,7 +1316,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E17" s="7" t="n"/>
+      <c r="E17" s="7" t="inlineStr"/>
       <c r="F17" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -1192,7 +1348,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E18" s="7" t="n"/>
+      <c r="E18" s="7" t="inlineStr"/>
       <c r="F18" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -1224,8 +1380,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
+      <c r="E19" s="7" t="inlineStr"/>
+      <c r="F19" s="7" t="inlineStr"/>
       <c r="G19" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -1233,16 +1389,36 @@
       </c>
       <c r="H19" s="7" t="inlineStr"/>
       <c r="I19" s="7" t="inlineStr"/>
-      <c r="J19" s="7" t="inlineStr"/>
-      <c r="K19" s="7" t="inlineStr"/>
-      <c r="L19" s="7" t="inlineStr"/>
-      <c r="M19" s="7" t="inlineStr"/>
-      <c r="N19" s="7" t="inlineStr"/>
-      <c r="O19" s="7" t="inlineStr"/>
-      <c r="P19" s="7" t="inlineStr"/>
-      <c r="Q19" s="7" t="inlineStr"/>
-      <c r="R19" s="7" t="inlineStr"/>
-      <c r="S19" s="7" t="inlineStr"/>
+      <c r="J19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="K19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="L19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="M19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="N19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="O19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="P19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="Q19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="R19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
+      <c r="S19" s="7" t="n">
+        <v>0.2313</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="7" t="inlineStr">
@@ -1261,7 +1437,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F20" s="7" t="n"/>
+      <c r="F20" s="7" t="inlineStr"/>
       <c r="G20" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -1269,16 +1445,36 @@
       </c>
       <c r="H20" s="7" t="inlineStr"/>
       <c r="I20" s="7" t="inlineStr"/>
-      <c r="J20" s="7" t="inlineStr"/>
-      <c r="K20" s="7" t="inlineStr"/>
-      <c r="L20" s="7" t="inlineStr"/>
-      <c r="M20" s="7" t="inlineStr"/>
-      <c r="N20" s="7" t="inlineStr"/>
-      <c r="O20" s="7" t="inlineStr"/>
-      <c r="P20" s="7" t="inlineStr"/>
-      <c r="Q20" s="7" t="inlineStr"/>
-      <c r="R20" s="7" t="inlineStr"/>
-      <c r="S20" s="7" t="inlineStr"/>
+      <c r="J20" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K20" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L20" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="M20" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="N20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="7" t="inlineStr">
@@ -1297,7 +1493,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F21" s="7" t="n"/>
+      <c r="F21" s="7" t="inlineStr"/>
       <c r="G21" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -1305,112 +1501,180 @@
       </c>
       <c r="H21" s="7" t="inlineStr"/>
       <c r="I21" s="7" t="inlineStr"/>
-      <c r="J21" s="7" t="inlineStr"/>
-      <c r="K21" s="7" t="inlineStr"/>
-      <c r="L21" s="7" t="inlineStr"/>
-      <c r="M21" s="7" t="inlineStr"/>
-      <c r="N21" s="7" t="inlineStr"/>
-      <c r="O21" s="7" t="inlineStr"/>
-      <c r="P21" s="7" t="inlineStr"/>
-      <c r="Q21" s="7" t="inlineStr"/>
-      <c r="R21" s="7" t="inlineStr"/>
-      <c r="S21" s="7" t="inlineStr"/>
+      <c r="J21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="N21" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="O21" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="P21" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q21" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="R21" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="S21" s="7" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="22">
-      <c r="B22" s="8" t="inlineStr">
-        <is>
-          <t>ind_steel_blafu_1</t>
-        </is>
-      </c>
-      <c r="C22" s="8" t="inlineStr"/>
-      <c r="D22" s="8" t="inlineStr">
-        <is>
-          <t>INPUT</t>
-        </is>
-      </c>
-      <c r="E22" s="8" t="inlineStr">
-        <is>
-          <t>sec_elec_ind</t>
-        </is>
-      </c>
-      <c r="F22" s="8" t="n"/>
-      <c r="G22" s="8" t="inlineStr"/>
-      <c r="H22" s="8" t="inlineStr"/>
-      <c r="I22" s="8" t="inlineStr"/>
-      <c r="J22" s="8" t="inlineStr"/>
-      <c r="K22" s="8" t="inlineStr"/>
-      <c r="L22" s="8" t="inlineStr"/>
-      <c r="M22" s="8" t="inlineStr"/>
-      <c r="N22" s="8" t="inlineStr"/>
-      <c r="O22" s="8" t="inlineStr"/>
-      <c r="P22" s="8" t="inlineStr"/>
-      <c r="Q22" s="8" t="inlineStr"/>
-      <c r="R22" s="8" t="inlineStr"/>
-      <c r="S22" s="8" t="inlineStr"/>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>ind_steel_blafu_0</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="inlineStr"/>
+      <c r="D22" s="7" t="inlineStr">
+        <is>
+          <t>NCAP_TLIFE</t>
+        </is>
+      </c>
+      <c r="E22" s="7" t="inlineStr"/>
+      <c r="F22" s="7" t="inlineStr"/>
+      <c r="G22" s="7" t="inlineStr"/>
+      <c r="H22" s="7" t="inlineStr"/>
+      <c r="I22" s="7" t="inlineStr"/>
+      <c r="J22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="K22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="L22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="M22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="N22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="O22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="P22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="R22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="S22" s="7" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="23">
-      <c r="B23" s="8" t="inlineStr">
-        <is>
-          <t>ind_steel_blafu_1</t>
-        </is>
-      </c>
-      <c r="C23" s="8" t="inlineStr"/>
-      <c r="D23" s="8" t="inlineStr">
-        <is>
-          <t>INPUT</t>
-        </is>
-      </c>
-      <c r="E23" s="8" t="inlineStr">
-        <is>
-          <t>pri_coal</t>
-        </is>
-      </c>
-      <c r="F23" s="8" t="n"/>
-      <c r="G23" s="8" t="inlineStr"/>
-      <c r="H23" s="8" t="inlineStr"/>
-      <c r="I23" s="8" t="inlineStr"/>
-      <c r="J23" s="8" t="inlineStr"/>
-      <c r="K23" s="8" t="inlineStr"/>
-      <c r="L23" s="8" t="inlineStr"/>
-      <c r="M23" s="8" t="inlineStr"/>
-      <c r="N23" s="8" t="inlineStr"/>
-      <c r="O23" s="8" t="inlineStr"/>
-      <c r="P23" s="8" t="inlineStr"/>
-      <c r="Q23" s="8" t="inlineStr"/>
-      <c r="R23" s="8" t="inlineStr"/>
-      <c r="S23" s="8" t="inlineStr"/>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>ind_steel_blafu_0</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr"/>
+      <c r="D23" s="7" t="inlineStr">
+        <is>
+          <t>PRC_RESID</t>
+        </is>
+      </c>
+      <c r="E23" s="7" t="inlineStr"/>
+      <c r="F23" s="7" t="inlineStr"/>
+      <c r="G23" s="7" t="inlineStr"/>
+      <c r="H23" s="7" t="inlineStr"/>
+      <c r="I23" s="7" t="inlineStr"/>
+      <c r="J23" s="7" t="n">
+        <v>31.462</v>
+      </c>
+      <c r="K23" s="7" t="n">
+        <v>27.85267695</v>
+      </c>
+      <c r="L23" s="7" t="n">
+        <v>22.28219805</v>
+      </c>
+      <c r="M23" s="7" t="n">
+        <v>16.7116485375</v>
+      </c>
+      <c r="N23" s="7" t="n">
+        <v>11.141099025</v>
+      </c>
+      <c r="O23" s="7" t="n">
+        <v>5.5705495125</v>
+      </c>
+      <c r="P23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="B24" s="8" t="inlineStr">
-        <is>
-          <t>ind_steel_blafu_1</t>
-        </is>
-      </c>
-      <c r="C24" s="8" t="inlineStr"/>
-      <c r="D24" s="8" t="inlineStr">
-        <is>
-          <t>INPUT</t>
-        </is>
-      </c>
-      <c r="E24" s="8" t="inlineStr">
-        <is>
-          <t>iip_coke</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="n"/>
-      <c r="G24" s="8" t="inlineStr"/>
-      <c r="H24" s="8" t="inlineStr"/>
-      <c r="I24" s="8" t="inlineStr"/>
-      <c r="J24" s="8" t="inlineStr"/>
-      <c r="K24" s="8" t="inlineStr"/>
-      <c r="L24" s="8" t="inlineStr"/>
-      <c r="M24" s="8" t="inlineStr"/>
-      <c r="N24" s="8" t="inlineStr"/>
-      <c r="O24" s="8" t="inlineStr"/>
-      <c r="P24" s="8" t="inlineStr"/>
-      <c r="Q24" s="8" t="inlineStr"/>
-      <c r="R24" s="8" t="inlineStr"/>
-      <c r="S24" s="8" t="inlineStr"/>
+      <c r="B24" s="7" t="inlineStr">
+        <is>
+          <t>ind_steel_blafu_0</t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr"/>
+      <c r="D24" s="7" t="inlineStr">
+        <is>
+          <t>NCAP_BND</t>
+        </is>
+      </c>
+      <c r="E24" s="7" t="inlineStr"/>
+      <c r="F24" s="7" t="inlineStr"/>
+      <c r="G24" s="7" t="inlineStr"/>
+      <c r="H24" s="7" t="inlineStr"/>
+      <c r="I24" s="7" t="inlineStr"/>
+      <c r="J24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="8" t="inlineStr">
@@ -1429,7 +1693,7 @@
           <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
-      <c r="F25" s="8" t="n"/>
+      <c r="F25" s="8" t="inlineStr"/>
       <c r="G25" s="8" t="inlineStr"/>
       <c r="H25" s="8" t="inlineStr"/>
       <c r="I25" s="8" t="inlineStr"/>
@@ -1461,7 +1725,7 @@
           <t>iip_steel_sinter</t>
         </is>
       </c>
-      <c r="F26" s="8" t="n"/>
+      <c r="F26" s="8" t="inlineStr"/>
       <c r="G26" s="8" t="inlineStr"/>
       <c r="H26" s="8" t="inlineStr"/>
       <c r="I26" s="8" t="inlineStr"/>
@@ -1493,7 +1757,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F27" s="8" t="n"/>
+      <c r="F27" s="8" t="inlineStr"/>
       <c r="G27" s="8" t="inlineStr"/>
       <c r="H27" s="8" t="inlineStr"/>
       <c r="I27" s="8" t="inlineStr"/>
@@ -1520,7 +1784,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E28" s="8" t="n"/>
+      <c r="E28" s="8" t="inlineStr"/>
       <c r="F28" s="8" t="inlineStr">
         <is>
           <t>iip_steel_raw_iron</t>
@@ -1552,7 +1816,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E29" s="8" t="n"/>
+      <c r="E29" s="8" t="inlineStr"/>
       <c r="F29" s="8" t="inlineStr">
         <is>
           <t>iip_steel_blafu_slag</t>
@@ -1584,7 +1848,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E30" s="8" t="n"/>
+      <c r="E30" s="8" t="inlineStr"/>
       <c r="F30" s="8" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -1616,7 +1880,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E31" s="8" t="n"/>
+      <c r="E31" s="8" t="inlineStr"/>
       <c r="F31" s="8" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -1648,7 +1912,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E32" s="8" t="n"/>
+      <c r="E32" s="8" t="inlineStr"/>
       <c r="F32" s="8" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -1680,8 +1944,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E33" s="8" t="n"/>
-      <c r="F33" s="8" t="n"/>
+      <c r="E33" s="8" t="inlineStr"/>
+      <c r="F33" s="8" t="inlineStr"/>
       <c r="G33" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -1717,7 +1981,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F34" s="8" t="n"/>
+      <c r="F34" s="8" t="inlineStr"/>
       <c r="G34" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -1753,7 +2017,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F35" s="8" t="n"/>
+      <c r="F35" s="8" t="inlineStr"/>
       <c r="G35" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -1789,7 +2053,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F36" s="7" t="n"/>
+      <c r="F36" s="7" t="inlineStr"/>
       <c r="G36" s="7" t="inlineStr"/>
       <c r="H36" s="7" t="inlineStr"/>
       <c r="I36" s="7" t="inlineStr"/>
@@ -1821,7 +2085,7 @@
           <t>pri_coal</t>
         </is>
       </c>
-      <c r="F37" s="7" t="n"/>
+      <c r="F37" s="7" t="inlineStr"/>
       <c r="G37" s="7" t="inlineStr"/>
       <c r="H37" s="7" t="inlineStr"/>
       <c r="I37" s="7" t="inlineStr"/>
@@ -1853,7 +2117,7 @@
           <t>iip_coke</t>
         </is>
       </c>
-      <c r="F38" s="7" t="n"/>
+      <c r="F38" s="7" t="inlineStr"/>
       <c r="G38" s="7" t="inlineStr"/>
       <c r="H38" s="7" t="inlineStr"/>
       <c r="I38" s="7" t="inlineStr"/>
@@ -1885,7 +2149,7 @@
           <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
-      <c r="F39" s="7" t="n"/>
+      <c r="F39" s="7" t="inlineStr"/>
       <c r="G39" s="7" t="inlineStr"/>
       <c r="H39" s="7" t="inlineStr"/>
       <c r="I39" s="7" t="inlineStr"/>
@@ -1917,7 +2181,7 @@
           <t>iip_steel_sinter</t>
         </is>
       </c>
-      <c r="F40" s="7" t="n"/>
+      <c r="F40" s="7" t="inlineStr"/>
       <c r="G40" s="7" t="inlineStr"/>
       <c r="H40" s="7" t="inlineStr"/>
       <c r="I40" s="7" t="inlineStr"/>
@@ -1949,7 +2213,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F41" s="7" t="n"/>
+      <c r="F41" s="7" t="inlineStr"/>
       <c r="G41" s="7" t="inlineStr"/>
       <c r="H41" s="7" t="inlineStr"/>
       <c r="I41" s="7" t="inlineStr"/>
@@ -1976,7 +2240,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E42" s="7" t="n"/>
+      <c r="E42" s="7" t="inlineStr"/>
       <c r="F42" s="7" t="inlineStr">
         <is>
           <t>iip_steel_raw_iron</t>
@@ -2008,7 +2272,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E43" s="7" t="n"/>
+      <c r="E43" s="7" t="inlineStr"/>
       <c r="F43" s="7" t="inlineStr">
         <is>
           <t>iip_steel_blafu_slag</t>
@@ -2040,7 +2304,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E44" s="7" t="n"/>
+      <c r="E44" s="7" t="inlineStr"/>
       <c r="F44" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -2072,7 +2336,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E45" s="7" t="n"/>
+      <c r="E45" s="7" t="inlineStr"/>
       <c r="F45" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -2104,7 +2368,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E46" s="7" t="n"/>
+      <c r="E46" s="7" t="inlineStr"/>
       <c r="F46" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -2136,8 +2400,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E47" s="7" t="n"/>
-      <c r="F47" s="7" t="n"/>
+      <c r="E47" s="7" t="inlineStr"/>
+      <c r="F47" s="7" t="inlineStr"/>
       <c r="G47" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2173,7 +2437,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F48" s="7" t="n"/>
+      <c r="F48" s="7" t="inlineStr"/>
       <c r="G48" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2209,7 +2473,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F49" s="7" t="n"/>
+      <c r="F49" s="7" t="inlineStr"/>
       <c r="G49" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2245,7 +2509,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F50" s="8" t="n"/>
+      <c r="F50" s="8" t="inlineStr"/>
       <c r="G50" s="8" t="inlineStr"/>
       <c r="H50" s="8" t="inlineStr"/>
       <c r="I50" s="8" t="inlineStr"/>
@@ -2272,7 +2536,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E51" s="8" t="n"/>
+      <c r="E51" s="8" t="inlineStr"/>
       <c r="F51" s="8" t="inlineStr">
         <is>
           <t>iip_heat_proc</t>
@@ -2309,7 +2573,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F52" s="7" t="n"/>
+      <c r="F52" s="7" t="inlineStr"/>
       <c r="G52" s="7" t="inlineStr"/>
       <c r="H52" s="7" t="inlineStr"/>
       <c r="I52" s="7" t="inlineStr"/>
@@ -2341,7 +2605,7 @@
           <t>iip_heat_proc</t>
         </is>
       </c>
-      <c r="F53" s="7" t="n"/>
+      <c r="F53" s="7" t="inlineStr"/>
       <c r="G53" s="7" t="inlineStr"/>
       <c r="H53" s="7" t="inlineStr"/>
       <c r="I53" s="7" t="inlineStr"/>
@@ -2373,7 +2637,7 @@
           <t>iip_steel_crudesteel</t>
         </is>
       </c>
-      <c r="F54" s="7" t="n"/>
+      <c r="F54" s="7" t="inlineStr"/>
       <c r="G54" s="7" t="inlineStr"/>
       <c r="H54" s="7" t="inlineStr"/>
       <c r="I54" s="7" t="inlineStr"/>
@@ -2400,7 +2664,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E55" s="7" t="n"/>
+      <c r="E55" s="7" t="inlineStr"/>
       <c r="F55" s="7" t="inlineStr">
         <is>
           <t>exo_steel</t>
@@ -2432,7 +2696,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E56" s="7" t="n"/>
+      <c r="E56" s="7" t="inlineStr"/>
       <c r="F56" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -2464,7 +2728,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E57" s="7" t="n"/>
+      <c r="E57" s="7" t="inlineStr"/>
       <c r="F57" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -2496,7 +2760,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E58" s="7" t="n"/>
+      <c r="E58" s="7" t="inlineStr"/>
       <c r="F58" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -2528,8 +2792,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E59" s="7" t="n"/>
-      <c r="F59" s="7" t="n"/>
+      <c r="E59" s="7" t="inlineStr"/>
+      <c r="F59" s="7" t="inlineStr"/>
       <c r="G59" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2565,7 +2829,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F60" s="7" t="n"/>
+      <c r="F60" s="7" t="inlineStr"/>
       <c r="G60" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2601,7 +2865,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F61" s="7" t="n"/>
+      <c r="F61" s="7" t="inlineStr"/>
       <c r="G61" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2637,7 +2901,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F62" s="8" t="n"/>
+      <c r="F62" s="8" t="inlineStr"/>
       <c r="G62" s="8" t="inlineStr"/>
       <c r="H62" s="8" t="inlineStr"/>
       <c r="I62" s="8" t="inlineStr"/>
@@ -2669,7 +2933,7 @@
           <t>iip_heat_proc</t>
         </is>
       </c>
-      <c r="F63" s="8" t="n"/>
+      <c r="F63" s="8" t="inlineStr"/>
       <c r="G63" s="8" t="inlineStr"/>
       <c r="H63" s="8" t="inlineStr"/>
       <c r="I63" s="8" t="inlineStr"/>
@@ -2701,7 +2965,7 @@
           <t>iip_steel_crudesteel</t>
         </is>
       </c>
-      <c r="F64" s="8" t="n"/>
+      <c r="F64" s="8" t="inlineStr"/>
       <c r="G64" s="8" t="inlineStr"/>
       <c r="H64" s="8" t="inlineStr"/>
       <c r="I64" s="8" t="inlineStr"/>
@@ -2728,7 +2992,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E65" s="8" t="n"/>
+      <c r="E65" s="8" t="inlineStr"/>
       <c r="F65" s="8" t="inlineStr">
         <is>
           <t>exo_steel</t>
@@ -2760,7 +3024,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E66" s="8" t="n"/>
+      <c r="E66" s="8" t="inlineStr"/>
       <c r="F66" s="8" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -2792,7 +3056,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E67" s="8" t="n"/>
+      <c r="E67" s="8" t="inlineStr"/>
       <c r="F67" s="8" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -2824,7 +3088,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E68" s="8" t="n"/>
+      <c r="E68" s="8" t="inlineStr"/>
       <c r="F68" s="8" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -2856,8 +3120,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E69" s="8" t="n"/>
-      <c r="F69" s="8" t="n"/>
+      <c r="E69" s="8" t="inlineStr"/>
+      <c r="F69" s="8" t="inlineStr"/>
       <c r="G69" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2893,7 +3157,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F70" s="8" t="n"/>
+      <c r="F70" s="8" t="inlineStr"/>
       <c r="G70" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2929,7 +3193,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F71" s="8" t="n"/>
+      <c r="F71" s="8" t="inlineStr"/>
       <c r="G71" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -2965,7 +3229,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F72" s="7" t="n"/>
+      <c r="F72" s="7" t="inlineStr"/>
       <c r="G72" s="7" t="inlineStr"/>
       <c r="H72" s="7" t="inlineStr"/>
       <c r="I72" s="7" t="inlineStr"/>
@@ -2997,7 +3261,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F73" s="7" t="n"/>
+      <c r="F73" s="7" t="inlineStr"/>
       <c r="G73" s="7" t="inlineStr"/>
       <c r="H73" s="7" t="inlineStr"/>
       <c r="I73" s="7" t="inlineStr"/>
@@ -3029,7 +3293,7 @@
           <t>iip_steel_sponge_iron</t>
         </is>
       </c>
-      <c r="F74" s="7" t="n"/>
+      <c r="F74" s="7" t="inlineStr"/>
       <c r="G74" s="7" t="inlineStr"/>
       <c r="H74" s="7" t="inlineStr"/>
       <c r="I74" s="7" t="inlineStr"/>
@@ -3056,7 +3320,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E75" s="7" t="n"/>
+      <c r="E75" s="7" t="inlineStr"/>
       <c r="F75" s="7" t="inlineStr">
         <is>
           <t>iip_steel_crudesteel</t>
@@ -3088,7 +3352,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E76" s="7" t="n"/>
+      <c r="E76" s="7" t="inlineStr"/>
       <c r="F76" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -3120,7 +3384,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E77" s="7" t="n"/>
+      <c r="E77" s="7" t="inlineStr"/>
       <c r="F77" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -3152,7 +3416,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E78" s="7" t="n"/>
+      <c r="E78" s="7" t="inlineStr"/>
       <c r="F78" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -3184,8 +3448,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E79" s="7" t="n"/>
-      <c r="F79" s="7" t="n"/>
+      <c r="E79" s="7" t="inlineStr"/>
+      <c r="F79" s="7" t="inlineStr"/>
       <c r="G79" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3221,7 +3485,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F80" s="7" t="n"/>
+      <c r="F80" s="7" t="inlineStr"/>
       <c r="G80" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3257,7 +3521,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F81" s="7" t="n"/>
+      <c r="F81" s="7" t="inlineStr"/>
       <c r="G81" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3293,7 +3557,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F82" s="8" t="n"/>
+      <c r="F82" s="8" t="inlineStr"/>
       <c r="G82" s="8" t="inlineStr"/>
       <c r="H82" s="8" t="inlineStr"/>
       <c r="I82" s="8" t="inlineStr"/>
@@ -3325,7 +3589,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F83" s="8" t="n"/>
+      <c r="F83" s="8" t="inlineStr"/>
       <c r="G83" s="8" t="inlineStr"/>
       <c r="H83" s="8" t="inlineStr"/>
       <c r="I83" s="8" t="inlineStr"/>
@@ -3357,7 +3621,7 @@
           <t>iip_steel_scrap</t>
         </is>
       </c>
-      <c r="F84" s="8" t="n"/>
+      <c r="F84" s="8" t="inlineStr"/>
       <c r="G84" s="8" t="inlineStr"/>
       <c r="H84" s="8" t="inlineStr"/>
       <c r="I84" s="8" t="inlineStr"/>
@@ -3384,7 +3648,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E85" s="8" t="n"/>
+      <c r="E85" s="8" t="inlineStr"/>
       <c r="F85" s="8" t="inlineStr">
         <is>
           <t>iip_steel_crudesteel</t>
@@ -3416,7 +3680,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E86" s="8" t="n"/>
+      <c r="E86" s="8" t="inlineStr"/>
       <c r="F86" s="8" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -3448,7 +3712,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E87" s="8" t="n"/>
+      <c r="E87" s="8" t="inlineStr"/>
       <c r="F87" s="8" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -3480,7 +3744,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E88" s="8" t="n"/>
+      <c r="E88" s="8" t="inlineStr"/>
       <c r="F88" s="8" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -3512,8 +3776,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E89" s="8" t="n"/>
-      <c r="F89" s="8" t="n"/>
+      <c r="E89" s="8" t="inlineStr"/>
+      <c r="F89" s="8" t="inlineStr"/>
       <c r="G89" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3549,7 +3813,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F90" s="8" t="n"/>
+      <c r="F90" s="8" t="inlineStr"/>
       <c r="G90" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3585,7 +3849,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F91" s="8" t="n"/>
+      <c r="F91" s="8" t="inlineStr"/>
       <c r="G91" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3621,7 +3885,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F92" s="7" t="n"/>
+      <c r="F92" s="7" t="inlineStr"/>
       <c r="G92" s="7" t="inlineStr"/>
       <c r="H92" s="7" t="inlineStr"/>
       <c r="I92" s="7" t="inlineStr"/>
@@ -3653,7 +3917,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F93" s="7" t="n"/>
+      <c r="F93" s="7" t="inlineStr"/>
       <c r="G93" s="7" t="inlineStr"/>
       <c r="H93" s="7" t="inlineStr"/>
       <c r="I93" s="7" t="inlineStr"/>
@@ -3685,7 +3949,7 @@
           <t>iip_steel_scrap</t>
         </is>
       </c>
-      <c r="F94" s="7" t="n"/>
+      <c r="F94" s="7" t="inlineStr"/>
       <c r="G94" s="7" t="inlineStr"/>
       <c r="H94" s="7" t="inlineStr"/>
       <c r="I94" s="7" t="inlineStr"/>
@@ -3712,7 +3976,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E95" s="7" t="n"/>
+      <c r="E95" s="7" t="inlineStr"/>
       <c r="F95" s="7" t="inlineStr">
         <is>
           <t>iip_steel_crudesteel</t>
@@ -3744,7 +4008,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E96" s="7" t="n"/>
+      <c r="E96" s="7" t="inlineStr"/>
       <c r="F96" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -3776,7 +4040,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E97" s="7" t="n"/>
+      <c r="E97" s="7" t="inlineStr"/>
       <c r="F97" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -3808,7 +4072,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E98" s="7" t="n"/>
+      <c r="E98" s="7" t="inlineStr"/>
       <c r="F98" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -3840,8 +4104,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E99" s="7" t="n"/>
-      <c r="F99" s="7" t="n"/>
+      <c r="E99" s="7" t="inlineStr"/>
+      <c r="F99" s="7" t="inlineStr"/>
       <c r="G99" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3877,7 +4141,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F100" s="7" t="n"/>
+      <c r="F100" s="7" t="inlineStr"/>
       <c r="G100" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3913,7 +4177,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F101" s="7" t="n"/>
+      <c r="F101" s="7" t="inlineStr"/>
       <c r="G101" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -3949,7 +4213,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F102" s="8" t="n"/>
+      <c r="F102" s="8" t="inlineStr"/>
       <c r="G102" s="8" t="inlineStr"/>
       <c r="H102" s="8" t="inlineStr"/>
       <c r="I102" s="8" t="inlineStr"/>
@@ -3981,7 +4245,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F103" s="8" t="n"/>
+      <c r="F103" s="8" t="inlineStr"/>
       <c r="G103" s="8" t="inlineStr"/>
       <c r="H103" s="8" t="inlineStr"/>
       <c r="I103" s="8" t="inlineStr"/>
@@ -4013,7 +4277,7 @@
           <t>iip_steel_iron_ore</t>
         </is>
       </c>
-      <c r="F104" s="8" t="n"/>
+      <c r="F104" s="8" t="inlineStr"/>
       <c r="G104" s="8" t="inlineStr"/>
       <c r="H104" s="8" t="inlineStr"/>
       <c r="I104" s="8" t="inlineStr"/>
@@ -4040,7 +4304,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E105" s="8" t="n"/>
+      <c r="E105" s="8" t="inlineStr"/>
       <c r="F105" s="8" t="inlineStr">
         <is>
           <t>iip_steel_crudesteel</t>
@@ -4077,7 +4341,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F106" s="7" t="n"/>
+      <c r="F106" s="7" t="inlineStr"/>
       <c r="G106" s="7" t="inlineStr"/>
       <c r="H106" s="7" t="inlineStr"/>
       <c r="I106" s="7" t="inlineStr"/>
@@ -4109,7 +4373,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F107" s="7" t="n"/>
+      <c r="F107" s="7" t="inlineStr"/>
       <c r="G107" s="7" t="inlineStr"/>
       <c r="H107" s="7" t="inlineStr"/>
       <c r="I107" s="7" t="inlineStr"/>
@@ -4141,7 +4405,7 @@
           <t>iip_steel_raw_iron</t>
         </is>
       </c>
-      <c r="F108" s="7" t="n"/>
+      <c r="F108" s="7" t="inlineStr"/>
       <c r="G108" s="7" t="inlineStr"/>
       <c r="H108" s="7" t="inlineStr"/>
       <c r="I108" s="7" t="inlineStr"/>
@@ -4168,7 +4432,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E109" s="7" t="n"/>
+      <c r="E109" s="7" t="inlineStr"/>
       <c r="F109" s="7" t="inlineStr">
         <is>
           <t>iip_steel_crudesteel</t>
@@ -4200,7 +4464,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E110" s="7" t="n"/>
+      <c r="E110" s="7" t="inlineStr"/>
       <c r="F110" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -4232,7 +4496,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E111" s="7" t="n"/>
+      <c r="E111" s="7" t="inlineStr"/>
       <c r="F111" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -4264,7 +4528,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E112" s="7" t="n"/>
+      <c r="E112" s="7" t="inlineStr"/>
       <c r="F112" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -4296,8 +4560,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E113" s="7" t="n"/>
-      <c r="F113" s="7" t="n"/>
+      <c r="E113" s="7" t="inlineStr"/>
+      <c r="F113" s="7" t="inlineStr"/>
       <c r="G113" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -4333,7 +4597,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F114" s="7" t="n"/>
+      <c r="F114" s="7" t="inlineStr"/>
       <c r="G114" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -4369,7 +4633,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F115" s="7" t="n"/>
+      <c r="F115" s="7" t="inlineStr"/>
       <c r="G115" s="7" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -4405,7 +4669,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F116" s="8" t="n"/>
+      <c r="F116" s="8" t="inlineStr"/>
       <c r="G116" s="8" t="inlineStr"/>
       <c r="H116" s="8" t="inlineStr"/>
       <c r="I116" s="8" t="inlineStr"/>
@@ -4437,7 +4701,7 @@
           <t>iip_steel_oxygen</t>
         </is>
       </c>
-      <c r="F117" s="8" t="n"/>
+      <c r="F117" s="8" t="inlineStr"/>
       <c r="G117" s="8" t="inlineStr"/>
       <c r="H117" s="8" t="inlineStr"/>
       <c r="I117" s="8" t="inlineStr"/>
@@ -4469,7 +4733,7 @@
           <t>iip_steel_raw_iron</t>
         </is>
       </c>
-      <c r="F118" s="8" t="n"/>
+      <c r="F118" s="8" t="inlineStr"/>
       <c r="G118" s="8" t="inlineStr"/>
       <c r="H118" s="8" t="inlineStr"/>
       <c r="I118" s="8" t="inlineStr"/>
@@ -4496,7 +4760,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E119" s="8" t="n"/>
+      <c r="E119" s="8" t="inlineStr"/>
       <c r="F119" s="8" t="inlineStr">
         <is>
           <t>iip_steel_crudesteel</t>
@@ -4528,7 +4792,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E120" s="8" t="n"/>
+      <c r="E120" s="8" t="inlineStr"/>
       <c r="F120" s="8" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -4560,7 +4824,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E121" s="8" t="n"/>
+      <c r="E121" s="8" t="inlineStr"/>
       <c r="F121" s="8" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -4592,7 +4856,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E122" s="8" t="n"/>
+      <c r="E122" s="8" t="inlineStr"/>
       <c r="F122" s="8" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -4624,8 +4888,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E123" s="8" t="n"/>
-      <c r="F123" s="8" t="n"/>
+      <c r="E123" s="8" t="inlineStr"/>
+      <c r="F123" s="8" t="inlineStr"/>
       <c r="G123" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -4661,7 +4925,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F124" s="8" t="n"/>
+      <c r="F124" s="8" t="inlineStr"/>
       <c r="G124" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -4697,7 +4961,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F125" s="8" t="n"/>
+      <c r="F125" s="8" t="inlineStr"/>
       <c r="G125" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -4733,7 +4997,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F126" s="7" t="n"/>
+      <c r="F126" s="7" t="inlineStr"/>
       <c r="G126" s="7" t="inlineStr"/>
       <c r="H126" s="7" t="inlineStr"/>
       <c r="I126" s="7" t="inlineStr"/>
@@ -4765,7 +5029,7 @@
           <t>iip_coke</t>
         </is>
       </c>
-      <c r="F127" s="7" t="n"/>
+      <c r="F127" s="7" t="inlineStr"/>
       <c r="G127" s="7" t="inlineStr"/>
       <c r="H127" s="7" t="inlineStr"/>
       <c r="I127" s="7" t="inlineStr"/>
@@ -4797,7 +5061,7 @@
           <t>iip_steel_iron_ore</t>
         </is>
       </c>
-      <c r="F128" s="7" t="n"/>
+      <c r="F128" s="7" t="inlineStr"/>
       <c r="G128" s="7" t="inlineStr"/>
       <c r="H128" s="7" t="inlineStr"/>
       <c r="I128" s="7" t="inlineStr"/>
@@ -4824,7 +5088,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E129" s="7" t="n"/>
+      <c r="E129" s="7" t="inlineStr"/>
       <c r="F129" s="7" t="inlineStr">
         <is>
           <t>iip_steel_iron_pellets</t>
@@ -4856,7 +5120,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E130" s="7" t="n"/>
+      <c r="E130" s="7" t="inlineStr"/>
       <c r="F130" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -4888,7 +5152,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E131" s="7" t="n"/>
+      <c r="E131" s="7" t="inlineStr"/>
       <c r="F131" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -4920,7 +5184,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E132" s="7" t="n"/>
+      <c r="E132" s="7" t="inlineStr"/>
       <c r="F132" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -4957,7 +5221,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F133" s="8" t="n"/>
+      <c r="F133" s="8" t="inlineStr"/>
       <c r="G133" s="8" t="inlineStr"/>
       <c r="H133" s="8" t="inlineStr"/>
       <c r="I133" s="8" t="inlineStr"/>
@@ -4989,7 +5253,7 @@
           <t>iip_steel_iron_ore</t>
         </is>
       </c>
-      <c r="F134" s="8" t="n"/>
+      <c r="F134" s="8" t="inlineStr"/>
       <c r="G134" s="8" t="inlineStr"/>
       <c r="H134" s="8" t="inlineStr"/>
       <c r="I134" s="8" t="inlineStr"/>
@@ -5016,7 +5280,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E135" s="8" t="n"/>
+      <c r="E135" s="8" t="inlineStr"/>
       <c r="F135" s="8" t="inlineStr">
         <is>
           <t>iip_steel_sinter</t>
@@ -5048,7 +5312,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E136" s="8" t="n"/>
+      <c r="E136" s="8" t="inlineStr"/>
       <c r="F136" s="8" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -5080,7 +5344,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E137" s="8" t="n"/>
+      <c r="E137" s="8" t="inlineStr"/>
       <c r="F137" s="8" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -5112,7 +5376,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E138" s="8" t="n"/>
+      <c r="E138" s="8" t="inlineStr"/>
       <c r="F138" s="8" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -5144,8 +5408,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E139" s="8" t="n"/>
-      <c r="F139" s="8" t="n"/>
+      <c r="E139" s="8" t="inlineStr"/>
+      <c r="F139" s="8" t="inlineStr"/>
       <c r="G139" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen_coal</t>
@@ -5181,7 +5445,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F140" s="8" t="n"/>
+      <c r="F140" s="8" t="inlineStr"/>
       <c r="G140" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen_coal</t>
@@ -5217,7 +5481,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F141" s="8" t="n"/>
+      <c r="F141" s="8" t="inlineStr"/>
       <c r="G141" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen_coal</t>
@@ -5253,7 +5517,7 @@
           <t>pri_coal</t>
         </is>
       </c>
-      <c r="F142" s="8" t="n"/>
+      <c r="F142" s="8" t="inlineStr"/>
       <c r="G142" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen_coal</t>
@@ -5289,7 +5553,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F143" s="7" t="n"/>
+      <c r="F143" s="7" t="inlineStr"/>
       <c r="G143" s="7" t="inlineStr"/>
       <c r="H143" s="7" t="inlineStr"/>
       <c r="I143" s="7" t="inlineStr"/>
@@ -5321,7 +5585,7 @@
           <t>pri_coal</t>
         </is>
       </c>
-      <c r="F144" s="7" t="n"/>
+      <c r="F144" s="7" t="inlineStr"/>
       <c r="G144" s="7" t="inlineStr"/>
       <c r="H144" s="7" t="inlineStr"/>
       <c r="I144" s="7" t="inlineStr"/>
@@ -5353,7 +5617,7 @@
           <t>iip_steel_iron_ore</t>
         </is>
       </c>
-      <c r="F145" s="7" t="n"/>
+      <c r="F145" s="7" t="inlineStr"/>
       <c r="G145" s="7" t="inlineStr"/>
       <c r="H145" s="7" t="inlineStr"/>
       <c r="I145" s="7" t="inlineStr"/>
@@ -5380,7 +5644,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E146" s="7" t="n"/>
+      <c r="E146" s="7" t="inlineStr"/>
       <c r="F146" s="7" t="inlineStr">
         <is>
           <t>iip_steel_sinter</t>
@@ -5412,7 +5676,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E147" s="7" t="n"/>
+      <c r="E147" s="7" t="inlineStr"/>
       <c r="F147" s="7" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -5444,7 +5708,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E148" s="7" t="n"/>
+      <c r="E148" s="7" t="inlineStr"/>
       <c r="F148" s="7" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -5476,7 +5740,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E149" s="7" t="n"/>
+      <c r="E149" s="7" t="inlineStr"/>
       <c r="F149" s="7" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -5513,7 +5777,7 @@
           <t>sec_elec_ind</t>
         </is>
       </c>
-      <c r="F150" s="8" t="n"/>
+      <c r="F150" s="8" t="inlineStr"/>
       <c r="G150" s="8" t="inlineStr"/>
       <c r="H150" s="8" t="inlineStr"/>
       <c r="I150" s="8" t="inlineStr"/>
@@ -5545,7 +5809,7 @@
           <t>iip_steel_iron_ore</t>
         </is>
       </c>
-      <c r="F151" s="8" t="n"/>
+      <c r="F151" s="8" t="inlineStr"/>
       <c r="G151" s="8" t="inlineStr"/>
       <c r="H151" s="8" t="inlineStr"/>
       <c r="I151" s="8" t="inlineStr"/>
@@ -5577,7 +5841,7 @@
           <t>iip_steel_iron_pellets</t>
         </is>
       </c>
-      <c r="F152" s="8" t="n"/>
+      <c r="F152" s="8" t="inlineStr"/>
       <c r="G152" s="8" t="inlineStr"/>
       <c r="H152" s="8" t="inlineStr"/>
       <c r="I152" s="8" t="inlineStr"/>
@@ -5604,7 +5868,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E153" s="8" t="n"/>
+      <c r="E153" s="8" t="inlineStr"/>
       <c r="F153" s="8" t="inlineStr">
         <is>
           <t>iip_steel_sponge_iron</t>
@@ -5636,7 +5900,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E154" s="8" t="n"/>
+      <c r="E154" s="8" t="inlineStr"/>
       <c r="F154" s="8" t="inlineStr">
         <is>
           <t>emi_CO2_f_ind</t>
@@ -5668,7 +5932,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E155" s="8" t="n"/>
+      <c r="E155" s="8" t="inlineStr"/>
       <c r="F155" s="8" t="inlineStr">
         <is>
           <t>emi_CH4_f_ind</t>
@@ -5700,7 +5964,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E156" s="8" t="n"/>
+      <c r="E156" s="8" t="inlineStr"/>
       <c r="F156" s="8" t="inlineStr">
         <is>
           <t>emi_N2O_f_ind</t>
@@ -5732,8 +5996,8 @@
           <t>ACT_EFF</t>
         </is>
       </c>
-      <c r="E157" s="8" t="n"/>
-      <c r="F157" s="8" t="n"/>
+      <c r="E157" s="8" t="inlineStr"/>
+      <c r="F157" s="8" t="inlineStr"/>
       <c r="G157" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -5769,7 +6033,7 @@
           <t>sec_methane</t>
         </is>
       </c>
-      <c r="F158" s="8" t="n"/>
+      <c r="F158" s="8" t="inlineStr"/>
       <c r="G158" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -5805,7 +6069,7 @@
           <t>sec_hydrogen</t>
         </is>
       </c>
-      <c r="F159" s="8" t="n"/>
+      <c r="F159" s="8" t="inlineStr"/>
       <c r="G159" s="8" t="inlineStr">
         <is>
           <t>cg_methane_hydrogen</t>
@@ -5841,7 +6105,7 @@
           <t>sec_biogas</t>
         </is>
       </c>
-      <c r="F160" s="7" t="n"/>
+      <c r="F160" s="7" t="inlineStr"/>
       <c r="G160" s="7" t="inlineStr"/>
       <c r="H160" s="7" t="inlineStr"/>
       <c r="I160" s="7" t="inlineStr"/>
@@ -5868,7 +6132,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E161" s="7" t="n"/>
+      <c r="E161" s="7" t="inlineStr"/>
       <c r="F161" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -5905,7 +6169,7 @@
           <t>sec_heating_oil</t>
         </is>
       </c>
-      <c r="F162" s="8" t="n"/>
+      <c r="F162" s="8" t="inlineStr"/>
       <c r="G162" s="8" t="inlineStr"/>
       <c r="H162" s="8" t="inlineStr"/>
       <c r="I162" s="8" t="inlineStr"/>
@@ -5932,7 +6196,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E163" s="8" t="n"/>
+      <c r="E163" s="8" t="inlineStr"/>
       <c r="F163" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -5964,7 +6228,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E164" s="8" t="n"/>
+      <c r="E164" s="8" t="inlineStr"/>
       <c r="F164" s="8" t="inlineStr">
         <is>
           <t>CO2_f_pow</t>
@@ -6001,7 +6265,7 @@
           <t>sec_H2</t>
         </is>
       </c>
-      <c r="F165" s="7" t="n"/>
+      <c r="F165" s="7" t="inlineStr"/>
       <c r="G165" s="7" t="inlineStr"/>
       <c r="H165" s="7" t="inlineStr"/>
       <c r="I165" s="7" t="inlineStr"/>
@@ -6028,7 +6292,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E166" s="7" t="n"/>
+      <c r="E166" s="7" t="inlineStr"/>
       <c r="F166" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6065,7 +6329,7 @@
           <t>pri_natural_gas</t>
         </is>
       </c>
-      <c r="F167" s="8" t="n"/>
+      <c r="F167" s="8" t="inlineStr"/>
       <c r="G167" s="8" t="inlineStr"/>
       <c r="H167" s="8" t="inlineStr"/>
       <c r="I167" s="8" t="inlineStr"/>
@@ -6092,7 +6356,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E168" s="8" t="n"/>
+      <c r="E168" s="8" t="inlineStr"/>
       <c r="F168" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6124,7 +6388,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E169" s="8" t="n"/>
+      <c r="E169" s="8" t="inlineStr"/>
       <c r="F169" s="8" t="inlineStr">
         <is>
           <t>CO2_f_pow</t>
@@ -6161,7 +6425,7 @@
           <t>sec_natural_gas_syn</t>
         </is>
       </c>
-      <c r="F170" s="7" t="n"/>
+      <c r="F170" s="7" t="inlineStr"/>
       <c r="G170" s="7" t="inlineStr"/>
       <c r="H170" s="7" t="inlineStr"/>
       <c r="I170" s="7" t="inlineStr"/>
@@ -6188,7 +6452,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E171" s="7" t="n"/>
+      <c r="E171" s="7" t="inlineStr"/>
       <c r="F171" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6220,7 +6484,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E172" s="7" t="n"/>
+      <c r="E172" s="7" t="inlineStr"/>
       <c r="F172" s="7" t="inlineStr">
         <is>
           <t>CO2_f_pow</t>
@@ -6257,7 +6521,7 @@
           <t>pri_biomass</t>
         </is>
       </c>
-      <c r="F173" s="8" t="n"/>
+      <c r="F173" s="8" t="inlineStr"/>
       <c r="G173" s="8" t="inlineStr"/>
       <c r="H173" s="8" t="inlineStr"/>
       <c r="I173" s="8" t="inlineStr"/>
@@ -6284,7 +6548,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E174" s="8" t="n"/>
+      <c r="E174" s="8" t="inlineStr"/>
       <c r="F174" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6321,7 +6585,7 @@
           <t>pri_coal</t>
         </is>
       </c>
-      <c r="F175" s="7" t="n"/>
+      <c r="F175" s="7" t="inlineStr"/>
       <c r="G175" s="7" t="inlineStr"/>
       <c r="H175" s="7" t="inlineStr"/>
       <c r="I175" s="7" t="inlineStr"/>
@@ -6348,7 +6612,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E176" s="7" t="n"/>
+      <c r="E176" s="7" t="inlineStr"/>
       <c r="F176" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6380,7 +6644,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E177" s="7" t="n"/>
+      <c r="E177" s="7" t="inlineStr"/>
       <c r="F177" s="7" t="inlineStr">
         <is>
           <t>CO2_f_pow</t>
@@ -6417,7 +6681,7 @@
           <t>sec_heating_oil</t>
         </is>
       </c>
-      <c r="F178" s="8" t="n"/>
+      <c r="F178" s="8" t="inlineStr"/>
       <c r="G178" s="8" t="inlineStr"/>
       <c r="H178" s="8" t="inlineStr"/>
       <c r="I178" s="8" t="inlineStr"/>
@@ -6444,7 +6708,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E179" s="8" t="n"/>
+      <c r="E179" s="8" t="inlineStr"/>
       <c r="F179" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6476,7 +6740,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E180" s="8" t="n"/>
+      <c r="E180" s="8" t="inlineStr"/>
       <c r="F180" s="8" t="inlineStr">
         <is>
           <t>CO2_f_pow</t>
@@ -6513,7 +6777,7 @@
           <t>pri_natural_gas</t>
         </is>
       </c>
-      <c r="F181" s="7" t="n"/>
+      <c r="F181" s="7" t="inlineStr"/>
       <c r="G181" s="7" t="inlineStr"/>
       <c r="H181" s="7" t="inlineStr"/>
       <c r="I181" s="7" t="inlineStr"/>
@@ -6540,7 +6804,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E182" s="7" t="n"/>
+      <c r="E182" s="7" t="inlineStr"/>
       <c r="F182" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6572,7 +6836,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E183" s="7" t="n"/>
+      <c r="E183" s="7" t="inlineStr"/>
       <c r="F183" s="7" t="inlineStr">
         <is>
           <t>CO2_f_pow</t>
@@ -6609,7 +6873,7 @@
           <t>pri_waste</t>
         </is>
       </c>
-      <c r="F184" s="8" t="n"/>
+      <c r="F184" s="8" t="inlineStr"/>
       <c r="G184" s="8" t="inlineStr"/>
       <c r="H184" s="8" t="inlineStr"/>
       <c r="I184" s="8" t="inlineStr"/>
@@ -6636,7 +6900,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E185" s="8" t="n"/>
+      <c r="E185" s="8" t="inlineStr"/>
       <c r="F185" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6668,7 +6932,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E186" s="8" t="n"/>
+      <c r="E186" s="8" t="inlineStr"/>
       <c r="F186" s="8" t="inlineStr">
         <is>
           <t>CO2_f_pow</t>
@@ -6705,7 +6969,7 @@
           <t>pri_geoth_heat</t>
         </is>
       </c>
-      <c r="F187" s="7" t="n"/>
+      <c r="F187" s="7" t="inlineStr"/>
       <c r="G187" s="7" t="inlineStr"/>
       <c r="H187" s="7" t="inlineStr"/>
       <c r="I187" s="7" t="inlineStr"/>
@@ -6732,7 +6996,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E188" s="7" t="n"/>
+      <c r="E188" s="7" t="inlineStr"/>
       <c r="F188" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6769,7 +7033,7 @@
           <t>pri_geoth_heat</t>
         </is>
       </c>
-      <c r="F189" s="8" t="n"/>
+      <c r="F189" s="8" t="inlineStr"/>
       <c r="G189" s="8" t="inlineStr"/>
       <c r="H189" s="8" t="inlineStr"/>
       <c r="I189" s="8" t="inlineStr"/>
@@ -6796,7 +7060,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E190" s="8" t="n"/>
+      <c r="E190" s="8" t="inlineStr"/>
       <c r="F190" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6828,7 +7092,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E191" s="8" t="n"/>
+      <c r="E191" s="8" t="inlineStr"/>
       <c r="F191" s="8" t="inlineStr">
         <is>
           <t>sec_heat_low</t>
@@ -6865,7 +7129,7 @@
           <t>pri_geoth_heat</t>
         </is>
       </c>
-      <c r="F192" s="7" t="n"/>
+      <c r="F192" s="7" t="inlineStr"/>
       <c r="G192" s="7" t="inlineStr"/>
       <c r="H192" s="7" t="inlineStr"/>
       <c r="I192" s="7" t="inlineStr"/>
@@ -6892,7 +7156,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E193" s="7" t="n"/>
+      <c r="E193" s="7" t="inlineStr"/>
       <c r="F193" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6929,7 +7193,7 @@
           <t>pri_geoth_heat</t>
         </is>
       </c>
-      <c r="F194" s="8" t="n"/>
+      <c r="F194" s="8" t="inlineStr"/>
       <c r="G194" s="8" t="inlineStr"/>
       <c r="H194" s="8" t="inlineStr"/>
       <c r="I194" s="8" t="inlineStr"/>
@@ -6956,7 +7220,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E195" s="8" t="n"/>
+      <c r="E195" s="8" t="inlineStr"/>
       <c r="F195" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -6988,7 +7252,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E196" s="8" t="n"/>
+      <c r="E196" s="8" t="inlineStr"/>
       <c r="F196" s="8" t="inlineStr">
         <is>
           <t>sec_heat_low</t>
@@ -7025,7 +7289,7 @@
           <t>pri_hydro_energy</t>
         </is>
       </c>
-      <c r="F197" s="7" t="n"/>
+      <c r="F197" s="7" t="inlineStr"/>
       <c r="G197" s="7" t="inlineStr"/>
       <c r="H197" s="7" t="inlineStr"/>
       <c r="I197" s="7" t="inlineStr"/>
@@ -7052,7 +7316,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E198" s="7" t="n"/>
+      <c r="E198" s="7" t="inlineStr"/>
       <c r="F198" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7089,7 +7353,7 @@
           <t>pri_hydro_energy</t>
         </is>
       </c>
-      <c r="F199" s="8" t="n"/>
+      <c r="F199" s="8" t="inlineStr"/>
       <c r="G199" s="8" t="inlineStr"/>
       <c r="H199" s="8" t="inlineStr"/>
       <c r="I199" s="8" t="inlineStr"/>
@@ -7116,7 +7380,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E200" s="8" t="n"/>
+      <c r="E200" s="8" t="inlineStr"/>
       <c r="F200" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7153,7 +7417,7 @@
           <t>pri_hydro_energy</t>
         </is>
       </c>
-      <c r="F201" s="7" t="n"/>
+      <c r="F201" s="7" t="inlineStr"/>
       <c r="G201" s="7" t="inlineStr"/>
       <c r="H201" s="7" t="inlineStr"/>
       <c r="I201" s="7" t="inlineStr"/>
@@ -7180,7 +7444,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E202" s="7" t="n"/>
+      <c r="E202" s="7" t="inlineStr"/>
       <c r="F202" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7217,7 +7481,7 @@
           <t>pri_uran</t>
         </is>
       </c>
-      <c r="F203" s="8" t="n"/>
+      <c r="F203" s="8" t="inlineStr"/>
       <c r="G203" s="8" t="inlineStr"/>
       <c r="H203" s="8" t="inlineStr"/>
       <c r="I203" s="8" t="inlineStr"/>
@@ -7244,7 +7508,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E204" s="8" t="n"/>
+      <c r="E204" s="8" t="inlineStr"/>
       <c r="F204" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7281,7 +7545,7 @@
           <t>pri_deuterium</t>
         </is>
       </c>
-      <c r="F205" s="7" t="n"/>
+      <c r="F205" s="7" t="inlineStr"/>
       <c r="G205" s="7" t="inlineStr"/>
       <c r="H205" s="7" t="inlineStr"/>
       <c r="I205" s="7" t="inlineStr"/>
@@ -7308,7 +7572,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E206" s="7" t="n"/>
+      <c r="E206" s="7" t="inlineStr"/>
       <c r="F206" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7345,7 +7609,7 @@
           <t>pri_solar_radiation</t>
         </is>
       </c>
-      <c r="F207" s="8" t="n"/>
+      <c r="F207" s="8" t="inlineStr"/>
       <c r="G207" s="8" t="inlineStr"/>
       <c r="H207" s="8" t="inlineStr"/>
       <c r="I207" s="8" t="inlineStr"/>
@@ -7372,7 +7636,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E208" s="8" t="n"/>
+      <c r="E208" s="8" t="inlineStr"/>
       <c r="F208" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7409,7 +7673,7 @@
           <t>pri_solar_radiation</t>
         </is>
       </c>
-      <c r="F209" s="7" t="n"/>
+      <c r="F209" s="7" t="inlineStr"/>
       <c r="G209" s="7" t="inlineStr"/>
       <c r="H209" s="7" t="inlineStr"/>
       <c r="I209" s="7" t="inlineStr"/>
@@ -7436,7 +7700,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E210" s="7" t="n"/>
+      <c r="E210" s="7" t="inlineStr"/>
       <c r="F210" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7473,7 +7737,7 @@
           <t>pri_solar_radiation</t>
         </is>
       </c>
-      <c r="F211" s="8" t="n"/>
+      <c r="F211" s="8" t="inlineStr"/>
       <c r="G211" s="8" t="inlineStr"/>
       <c r="H211" s="8" t="inlineStr"/>
       <c r="I211" s="8" t="inlineStr"/>
@@ -7500,7 +7764,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E212" s="8" t="n"/>
+      <c r="E212" s="8" t="inlineStr"/>
       <c r="F212" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7537,7 +7801,7 @@
           <t>sec_elec</t>
         </is>
       </c>
-      <c r="F213" s="7" t="n"/>
+      <c r="F213" s="7" t="inlineStr"/>
       <c r="G213" s="7" t="inlineStr"/>
       <c r="H213" s="7" t="inlineStr"/>
       <c r="I213" s="7" t="inlineStr"/>
@@ -7564,7 +7828,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E214" s="7" t="n"/>
+      <c r="E214" s="7" t="inlineStr"/>
       <c r="F214" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7601,7 +7865,7 @@
           <t>sec_elec</t>
         </is>
       </c>
-      <c r="F215" s="8" t="n"/>
+      <c r="F215" s="8" t="inlineStr"/>
       <c r="G215" s="8" t="inlineStr"/>
       <c r="H215" s="8" t="inlineStr"/>
       <c r="I215" s="8" t="inlineStr"/>
@@ -7628,7 +7892,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E216" s="8" t="n"/>
+      <c r="E216" s="8" t="inlineStr"/>
       <c r="F216" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7665,7 +7929,7 @@
           <t>sec_elec</t>
         </is>
       </c>
-      <c r="F217" s="7" t="n"/>
+      <c r="F217" s="7" t="inlineStr"/>
       <c r="G217" s="7" t="inlineStr"/>
       <c r="H217" s="7" t="inlineStr"/>
       <c r="I217" s="7" t="inlineStr"/>
@@ -7692,7 +7956,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E218" s="7" t="n"/>
+      <c r="E218" s="7" t="inlineStr"/>
       <c r="F218" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7729,7 +7993,7 @@
           <t>sec_elec</t>
         </is>
       </c>
-      <c r="F219" s="8" t="n"/>
+      <c r="F219" s="8" t="inlineStr"/>
       <c r="G219" s="8" t="inlineStr"/>
       <c r="H219" s="8" t="inlineStr"/>
       <c r="I219" s="8" t="inlineStr"/>
@@ -7756,7 +8020,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E220" s="8" t="n"/>
+      <c r="E220" s="8" t="inlineStr"/>
       <c r="F220" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7793,7 +8057,7 @@
           <t>sec_elec</t>
         </is>
       </c>
-      <c r="F221" s="7" t="n"/>
+      <c r="F221" s="7" t="inlineStr"/>
       <c r="G221" s="7" t="inlineStr"/>
       <c r="H221" s="7" t="inlineStr"/>
       <c r="I221" s="7" t="inlineStr"/>
@@ -7820,7 +8084,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E222" s="7" t="n"/>
+      <c r="E222" s="7" t="inlineStr"/>
       <c r="F222" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7857,7 +8121,7 @@
           <t>pri_wind_energy_off</t>
         </is>
       </c>
-      <c r="F223" s="8" t="n"/>
+      <c r="F223" s="8" t="inlineStr"/>
       <c r="G223" s="8" t="inlineStr"/>
       <c r="H223" s="8" t="inlineStr"/>
       <c r="I223" s="8" t="inlineStr"/>
@@ -7884,7 +8148,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E224" s="8" t="n"/>
+      <c r="E224" s="8" t="inlineStr"/>
       <c r="F224" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7921,7 +8185,7 @@
           <t>pri_wind_energy_off</t>
         </is>
       </c>
-      <c r="F225" s="7" t="n"/>
+      <c r="F225" s="7" t="inlineStr"/>
       <c r="G225" s="7" t="inlineStr"/>
       <c r="H225" s="7" t="inlineStr"/>
       <c r="I225" s="7" t="inlineStr"/>
@@ -7948,7 +8212,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E226" s="7" t="n"/>
+      <c r="E226" s="7" t="inlineStr"/>
       <c r="F226" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -7985,7 +8249,7 @@
           <t>pri_wind_energy_on</t>
         </is>
       </c>
-      <c r="F227" s="8" t="n"/>
+      <c r="F227" s="8" t="inlineStr"/>
       <c r="G227" s="8" t="inlineStr"/>
       <c r="H227" s="8" t="inlineStr"/>
       <c r="I227" s="8" t="inlineStr"/>
@@ -8012,7 +8276,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E228" s="8" t="n"/>
+      <c r="E228" s="8" t="inlineStr"/>
       <c r="F228" s="8" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -8049,7 +8313,7 @@
           <t>sec_H2</t>
         </is>
       </c>
-      <c r="F229" s="7" t="n"/>
+      <c r="F229" s="7" t="inlineStr"/>
       <c r="G229" s="7" t="inlineStr"/>
       <c r="H229" s="7" t="inlineStr"/>
       <c r="I229" s="7" t="inlineStr"/>
@@ -8081,7 +8345,7 @@
           <t>sec_heat_low</t>
         </is>
       </c>
-      <c r="F230" s="7" t="n"/>
+      <c r="F230" s="7" t="inlineStr"/>
       <c r="G230" s="7" t="inlineStr"/>
       <c r="H230" s="7" t="inlineStr"/>
       <c r="I230" s="7" t="inlineStr"/>
@@ -8108,7 +8372,7 @@
           <t>OUTPUT</t>
         </is>
       </c>
-      <c r="E231" s="7" t="n"/>
+      <c r="E231" s="7" t="inlineStr"/>
       <c r="F231" s="7" t="inlineStr">
         <is>
           <t>sec_elec</t>
@@ -10228,12 +10492,12 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>iip_steel_sinter</t>
+          <t>sec_hydrogen</t>
         </is>
       </c>
     </row>
@@ -10245,7 +10509,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sec_elec</t>
+          <t>sec_natural_gas_syn</t>
         </is>
       </c>
     </row>
@@ -10257,19 +10521,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>pri_wind_energy_on</t>
+          <t>pri_wind_energy_off</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>DEM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>iip_steel_sponge_iron</t>
+          <t>exo_steel</t>
         </is>
       </c>
     </row>
@@ -10281,19 +10545,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>iip_coke</t>
+          <t>iip_heat_proc</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>pri_natural_gas</t>
+          <t>iip_steel_sponge_iron</t>
         </is>
       </c>
     </row>
@@ -10305,43 +10569,43 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>pri_solar_radiation</t>
+          <t>pri_deuterium</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>pri_wind_energy_off</t>
+          <t>[emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>iip_steel_blafu_slag</t>
+          <t>iip_steel_iron_pellets</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>sec_heat_high</t>
+          <t>emi_CO2_f_ind</t>
         </is>
       </c>
     </row>
@@ -10353,19 +10617,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_reusable</t>
+          <t>emi_CO2_f_x2x_neg_stored]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>sec_hydrogen</t>
+          <t>emi_CO2_f_x2x</t>
         </is>
       </c>
     </row>
@@ -10377,7 +10641,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>sec_heavy_fuel_oil</t>
+          <t>CO2_f_pow</t>
         </is>
       </c>
     </row>
@@ -10389,19 +10653,19 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CO2_f_pow</t>
+          <t>iip_steel_blafu_slag</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[emi_CO2_f_x2x_neg_reusable</t>
+          <t>sec_heavy_fuel_oil</t>
         </is>
       </c>
     </row>
@@ -10413,7 +10677,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>sec_elec_ind</t>
+          <t>pri_wind_energy_on</t>
         </is>
       </c>
     </row>
@@ -10425,7 +10689,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>pri_waste</t>
+          <t>pri_hydro_energy</t>
         </is>
       </c>
     </row>
@@ -10437,7 +10701,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>pri_biomass</t>
+          <t>sec_elec</t>
         </is>
       </c>
     </row>
@@ -10473,19 +10737,19 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>pri_uran</t>
+          <t>sec_biogas</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>iip_steel_scrap</t>
+          <t>pri_geoth_heat</t>
         </is>
       </c>
     </row>
@@ -10497,31 +10761,31 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x_neg_stored]</t>
+          <t>emi_N2O_f_ind</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>emi_CO2_f_ind</t>
+          <t>iip_steel_iron_ore</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>iip_steel_raw_iron</t>
+          <t>pri_solar_radiation</t>
         </is>
       </c>
     </row>
@@ -10533,7 +10797,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>sec_methane</t>
+          <t>sec_heat_high</t>
         </is>
       </c>
     </row>
@@ -10545,19 +10809,19 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>iip_heat_proc</t>
+          <t>sec_methane</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>emi_CH4_f_ind</t>
+          <t>iip_coke</t>
         </is>
       </c>
     </row>
@@ -10569,7 +10833,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>pri_crude_oil</t>
+          <t>sec_H2</t>
         </is>
       </c>
     </row>
@@ -10581,43 +10845,43 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>sec_natural_gas_syn</t>
+          <t>pri_coal</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>emi_CO2_f_x2x</t>
+          <t>pri_crude_oil</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>iip_steel_oxygen</t>
+          <t>emi_CH4_f_ind</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>sec_H2</t>
+          <t>iip_steel_oxygen</t>
         </is>
       </c>
     </row>
@@ -10629,19 +10893,19 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>sec_biogas</t>
+          <t>sec_heating_oil</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>pri_coal</t>
+          <t>iip_steel_sinter</t>
         </is>
       </c>
     </row>
@@ -10653,7 +10917,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>sec_heating_oil</t>
+          <t>sec_elec_ind</t>
         </is>
       </c>
     </row>
@@ -10665,19 +10929,19 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>pri_geoth_heat</t>
+          <t>pri_natural_gas</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>ENV</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>pri_deuterium</t>
+          <t>emi_CO2_f_x2x_neg_reusable</t>
         </is>
       </c>
     </row>
@@ -10689,55 +10953,55 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>iip_steel_iron_pellets</t>
+          <t>iip_steel_raw_iron</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>DEM</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>exo_steel</t>
+          <t>pri_uran</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>MAT</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>iip_steel_iron_ore</t>
+          <t>pri_biomass</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>ENV</t>
+          <t>NRG</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>emi_N2O_f_ind</t>
+          <t>pri_waste</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>NRG</t>
+          <t>MAT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>pri_hydro_energy</t>
+          <t>iip_steel_scrap</t>
         </is>
       </c>
     </row>

</xml_diff>